<commit_message>
chg: Added F-16 presets, added links to TGT list (Tgt folders)
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAC Joint Target List.xlsx
+++ b/INTELLIGENCE/OPAC Joint Target List.xlsx
@@ -3254,7 +3254,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3530,7 +3530,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3611,6 +3610,7 @@
     <xf numFmtId="0" fontId="26" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3620,25 +3620,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3652,17 +3647,22 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3681,7 +3681,8 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
@@ -3716,7 +3717,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3750,7 +3751,7 @@
         <xdr:cNvPr id="3" name="image2.png" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3789,7 +3790,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3823,7 +3824,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3862,7 +3863,7 @@
         <xdr:cNvPr id="2" name="image10.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3896,7 +3897,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3935,7 +3936,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4092,7 +4093,7 @@
         <xdr:cNvPr id="4" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4126,7 +4127,7 @@
         <xdr:cNvPr id="5" name="image6.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4165,7 +4166,7 @@
         <xdr:cNvPr id="4" name="Shape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4322,7 +4323,7 @@
         <xdr:cNvPr id="3" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4356,7 +4357,7 @@
         <xdr:cNvPr id="5" name="image9.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4395,7 +4396,7 @@
         <xdr:cNvPr id="5" name="Shape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4576,7 +4577,7 @@
         <xdr:cNvPr id="3" name="image7.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4610,7 +4611,7 @@
         <xdr:cNvPr id="4" name="image14.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4649,7 +4650,7 @@
         <xdr:cNvPr id="6" name="Shape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4770,7 +4771,7 @@
         <xdr:cNvPr id="3" name="image13.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4804,7 +4805,7 @@
         <xdr:cNvPr id="4" name="image11.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4838,7 +4839,7 @@
         <xdr:cNvPr id="5" name="image12.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5063,10 +5064,10 @@
   <dimension ref="A1:J998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E210" sqref="E210"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5133,7 +5134,7 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" ht="14.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="168" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="76" t="s">
@@ -5149,13 +5150,13 @@
       <c r="F4" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="104" t="s">
+      <c r="G4" s="103" t="s">
         <v>12</v>
       </c>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" ht="14.25">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="104" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="75" t="s">
@@ -5171,13 +5172,13 @@
       <c r="F5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="106" t="s">
+      <c r="G5" s="105" t="s">
         <v>16</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" ht="14.25">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="169" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="74" t="s">
@@ -5193,13 +5194,13 @@
       <c r="F6" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="108" t="s">
+      <c r="G6" s="107" t="s">
         <v>21</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="14.25">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="133" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="75" t="s">
@@ -5215,13 +5216,13 @@
       <c r="F7" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="105" t="s">
         <v>25</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" ht="14.25">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="106" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="74" t="s">
@@ -5237,13 +5238,13 @@
       <c r="F8" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="108" t="s">
+      <c r="G8" s="107" t="s">
         <v>29</v>
       </c>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" ht="14.25">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="104" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="75" t="s">
@@ -5261,13 +5262,13 @@
       <c r="F9" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="106" t="s">
+      <c r="G9" s="105" t="s">
         <v>648</v>
       </c>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" ht="14.25">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="106" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="74" t="s">
@@ -5285,13 +5286,13 @@
       <c r="F10" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="108" t="s">
+      <c r="G10" s="107" t="s">
         <v>648</v>
       </c>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" ht="14.25">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="104" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="75" t="s">
@@ -5309,13 +5310,13 @@
       <c r="F11" s="71" t="s">
         <v>665</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="105" t="s">
         <v>648</v>
       </c>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" ht="14.25">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="106" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="74" t="s">
@@ -5333,13 +5334,13 @@
       <c r="F12" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="108" t="s">
+      <c r="G12" s="107" t="s">
         <v>648</v>
       </c>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" ht="14.25">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="104" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="75" t="s">
@@ -5355,13 +5356,13 @@
       <c r="F13" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="105" t="s">
         <v>648</v>
       </c>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" ht="14.25">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="169" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="74" t="s">
@@ -5377,13 +5378,13 @@
       <c r="F14" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="108" t="s">
+      <c r="G14" s="107" t="s">
         <v>51</v>
       </c>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" ht="14.25">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="104" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="75" t="s">
@@ -5399,13 +5400,13 @@
       <c r="F15" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="106" t="s">
+      <c r="G15" s="105" t="s">
         <v>56</v>
       </c>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" ht="14.25">
-      <c r="A16" s="107" t="s">
+      <c r="A16" s="106" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="74" t="s">
@@ -5421,13 +5422,13 @@
       <c r="F16" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="108" t="s">
+      <c r="G16" s="107" t="s">
         <v>61</v>
       </c>
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" ht="14.25">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="104" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="75" t="s">
@@ -5443,13 +5444,13 @@
       <c r="F17" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="105" t="s">
         <v>66</v>
       </c>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" ht="14.25">
-      <c r="A18" s="107" t="s">
+      <c r="A18" s="106" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="74" t="s">
@@ -5465,13 +5466,13 @@
       <c r="F18" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="108" t="s">
+      <c r="G18" s="107" t="s">
         <v>71</v>
       </c>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" ht="14.25">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="104" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="75" t="s">
@@ -5487,13 +5488,13 @@
       <c r="F19" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="105" t="s">
         <v>76</v>
       </c>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" ht="14.25">
-      <c r="A20" s="107" t="s">
+      <c r="A20" s="106" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="74" t="s">
@@ -5509,13 +5510,13 @@
       <c r="F20" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="108" t="s">
+      <c r="G20" s="107" t="s">
         <v>80</v>
       </c>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="104" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="83" t="s">
@@ -5531,13 +5532,13 @@
       <c r="F21" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="106" t="s">
+      <c r="G21" s="105" t="s">
         <v>80</v>
       </c>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A22" s="107" t="s">
+      <c r="A22" s="106" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="74" t="s">
@@ -5553,13 +5554,13 @@
       <c r="F22" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="108" t="s">
+      <c r="G22" s="107" t="s">
         <v>89</v>
       </c>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="104" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="75" t="s">
@@ -5575,13 +5576,13 @@
       <c r="F23" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="106" t="s">
+      <c r="G23" s="105" t="s">
         <v>94</v>
       </c>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="106" t="s">
         <v>95</v>
       </c>
       <c r="B24" s="74" t="s">
@@ -5597,13 +5598,13 @@
       <c r="F24" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="108" t="s">
+      <c r="G24" s="107" t="s">
         <v>99</v>
       </c>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A25" s="105" t="s">
+      <c r="A25" s="104" t="s">
         <v>100</v>
       </c>
       <c r="B25" s="75" t="s">
@@ -5619,13 +5620,13 @@
       <c r="F25" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="106" t="s">
+      <c r="G25" s="105" t="s">
         <v>103</v>
       </c>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="106" t="s">
         <v>104</v>
       </c>
       <c r="B26" s="74" t="s">
@@ -5641,13 +5642,13 @@
       <c r="F26" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="108" t="s">
+      <c r="G26" s="107" t="s">
         <v>108</v>
       </c>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="105" t="s">
+      <c r="A27" s="104" t="s">
         <v>109</v>
       </c>
       <c r="B27" s="75" t="s">
@@ -5663,13 +5664,13 @@
       <c r="F27" s="71" t="s">
         <v>666</v>
       </c>
-      <c r="G27" s="106" t="s">
+      <c r="G27" s="105" t="s">
         <v>649</v>
       </c>
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="106" t="s">
         <v>112</v>
       </c>
       <c r="B28" s="74" t="s">
@@ -5685,13 +5686,13 @@
       <c r="F28" s="72" t="s">
         <v>663</v>
       </c>
-      <c r="G28" s="108" t="s">
+      <c r="G28" s="107" t="s">
         <v>651</v>
       </c>
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="104" t="s">
         <v>113</v>
       </c>
       <c r="B29" s="75" t="s">
@@ -5707,13 +5708,13 @@
       <c r="F29" s="71" t="s">
         <v>662</v>
       </c>
-      <c r="G29" s="106" t="s">
+      <c r="G29" s="105" t="s">
         <v>650</v>
       </c>
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="107" t="s">
+      <c r="A30" s="106" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="74" t="s">
@@ -5729,13 +5730,13 @@
       <c r="F30" s="72" t="s">
         <v>664</v>
       </c>
-      <c r="G30" s="108" t="s">
+      <c r="G30" s="107" t="s">
         <v>657</v>
       </c>
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="105" t="s">
+      <c r="A31" s="104" t="s">
         <v>116</v>
       </c>
       <c r="B31" s="75" t="s">
@@ -5751,13 +5752,13 @@
       <c r="F31" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="G31" s="106" t="s">
+      <c r="G31" s="105" t="s">
         <v>120</v>
       </c>
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="107" t="s">
+      <c r="A32" s="106" t="s">
         <v>121</v>
       </c>
       <c r="B32" s="74" t="s">
@@ -5773,13 +5774,13 @@
       <c r="F32" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="G32" s="108" t="s">
+      <c r="G32" s="107" t="s">
         <v>120</v>
       </c>
       <c r="J32"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="105" t="s">
+      <c r="A33" s="104" t="s">
         <v>124</v>
       </c>
       <c r="B33" s="75" t="s">
@@ -5795,13 +5796,13 @@
       <c r="F33" s="71" t="s">
         <v>658</v>
       </c>
-      <c r="G33" s="106" t="s">
+      <c r="G33" s="105" t="s">
         <v>659</v>
       </c>
       <c r="J33"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="108" t="s">
         <v>127</v>
       </c>
       <c r="B34" s="87" t="s">
@@ -5817,13 +5818,13 @@
       <c r="F34" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="G34" s="110" t="s">
+      <c r="G34" s="109" t="s">
         <v>131</v>
       </c>
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A35" s="105" t="s">
+      <c r="A35" s="104" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="75" t="s">
@@ -5839,13 +5840,13 @@
       <c r="F35" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="G35" s="106" t="s">
+      <c r="G35" s="105" t="s">
         <v>135</v>
       </c>
       <c r="J35"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="106" t="s">
         <v>136</v>
       </c>
       <c r="B36" s="74" t="s">
@@ -5861,13 +5862,13 @@
       <c r="F36" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="G36" s="108" t="s">
+      <c r="G36" s="107" t="s">
         <v>139</v>
       </c>
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="105" t="s">
+      <c r="A37" s="104" t="s">
         <v>140</v>
       </c>
       <c r="B37" s="75" t="s">
@@ -5883,37 +5884,37 @@
       <c r="F37" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="G37" s="106" t="s">
+      <c r="G37" s="105" t="s">
         <v>56</v>
       </c>
       <c r="J37"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="129" t="s">
+      <c r="A38" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="130" t="s">
+      <c r="B38" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="127" t="s">
+      <c r="C38" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="128" t="s">
+      <c r="D38" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="131" t="s">
+      <c r="E38" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="132" t="s">
+      <c r="F38" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="133" t="s">
+      <c r="G38" s="132" t="s">
         <v>7</v>
       </c>
       <c r="J38"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A39" s="107" t="s">
+      <c r="A39" s="106" t="s">
         <v>143</v>
       </c>
       <c r="B39" s="90" t="s">
@@ -5929,13 +5930,13 @@
       <c r="F39" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="G39" s="108" t="s">
+      <c r="G39" s="107" t="s">
         <v>146</v>
       </c>
       <c r="J39"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A40" s="105" t="s">
+      <c r="A40" s="104" t="s">
         <v>147</v>
       </c>
       <c r="B40" s="75" t="s">
@@ -5951,13 +5952,13 @@
       <c r="F40" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="G40" s="106" t="s">
+      <c r="G40" s="105" t="s">
         <v>150</v>
       </c>
       <c r="J40"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A41" s="107" t="s">
+      <c r="A41" s="106" t="s">
         <v>151</v>
       </c>
       <c r="B41" s="91" t="s">
@@ -5973,13 +5974,13 @@
       <c r="F41" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="108" t="s">
+      <c r="G41" s="107" t="s">
         <v>154</v>
       </c>
       <c r="J41"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A42" s="105" t="s">
+      <c r="A42" s="104" t="s">
         <v>155</v>
       </c>
       <c r="B42" s="75" t="s">
@@ -5995,13 +5996,13 @@
       <c r="F42" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="G42" s="106" t="s">
+      <c r="G42" s="105" t="s">
         <v>158</v>
       </c>
       <c r="J42"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A43" s="107" t="s">
+      <c r="A43" s="106" t="s">
         <v>159</v>
       </c>
       <c r="B43" s="74" t="s">
@@ -6017,13 +6018,13 @@
       <c r="F43" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="G43" s="108" t="s">
+      <c r="G43" s="107" t="s">
         <v>162</v>
       </c>
       <c r="J43"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A44" s="105" t="s">
+      <c r="A44" s="104" t="s">
         <v>163</v>
       </c>
       <c r="B44" s="75" t="s">
@@ -6039,13 +6040,13 @@
       <c r="F44" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="G44" s="106" t="s">
+      <c r="G44" s="105" t="s">
         <v>166</v>
       </c>
       <c r="J44"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A45" s="107" t="s">
+      <c r="A45" s="106" t="s">
         <v>167</v>
       </c>
       <c r="B45" s="74" t="s">
@@ -6061,13 +6062,13 @@
       <c r="F45" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="G45" s="108" t="s">
+      <c r="G45" s="107" t="s">
         <v>170</v>
       </c>
       <c r="J45"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A46" s="105" t="s">
+      <c r="A46" s="104" t="s">
         <v>171</v>
       </c>
       <c r="B46" s="75" t="s">
@@ -6083,13 +6084,13 @@
       <c r="F46" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="G46" s="106" t="s">
+      <c r="G46" s="105" t="s">
         <v>174</v>
       </c>
       <c r="J46"/>
     </row>
     <row r="47" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A47" s="107" t="s">
+      <c r="A47" s="106" t="s">
         <v>175</v>
       </c>
       <c r="B47" s="74" t="s">
@@ -6105,13 +6106,13 @@
       <c r="F47" s="72" t="s">
         <v>177</v>
       </c>
-      <c r="G47" s="108" t="s">
+      <c r="G47" s="107" t="s">
         <v>178</v>
       </c>
       <c r="J47"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="104" t="s">
         <v>179</v>
       </c>
       <c r="B48" s="82" t="s">
@@ -6127,13 +6128,13 @@
       <c r="F48" s="71" t="s">
         <v>670</v>
       </c>
-      <c r="G48" s="106" t="s">
+      <c r="G48" s="105" t="s">
         <v>669</v>
       </c>
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A49" s="107" t="s">
+      <c r="A49" s="106" t="s">
         <v>180</v>
       </c>
       <c r="B49" s="74" t="s">
@@ -6149,13 +6150,13 @@
       <c r="F49" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="G49" s="108" t="s">
+      <c r="G49" s="107" t="s">
         <v>740</v>
       </c>
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A50" s="105" t="s">
+      <c r="A50" s="104" t="s">
         <v>183</v>
       </c>
       <c r="B50" s="75" t="s">
@@ -6171,13 +6172,13 @@
       <c r="F50" s="71" t="s">
         <v>184</v>
       </c>
-      <c r="G50" s="106" t="s">
+      <c r="G50" s="105" t="s">
         <v>741</v>
       </c>
       <c r="J50"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A51" s="107" t="s">
+      <c r="A51" s="106" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="74" t="s">
@@ -6193,13 +6194,13 @@
       <c r="F51" s="72" t="s">
         <v>187</v>
       </c>
-      <c r="G51" s="108" t="s">
+      <c r="G51" s="107" t="s">
         <v>742</v>
       </c>
       <c r="J51"/>
     </row>
     <row r="52" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A52" s="105" t="s">
+      <c r="A52" s="104" t="s">
         <v>188</v>
       </c>
       <c r="B52" s="75" t="s">
@@ -6215,13 +6216,13 @@
       <c r="F52" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="G52" s="106" t="s">
+      <c r="G52" s="105" t="s">
         <v>743</v>
       </c>
       <c r="J52"/>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A53" s="107" t="s">
+      <c r="A53" s="106" t="s">
         <v>191</v>
       </c>
       <c r="B53" s="74" t="s">
@@ -6237,13 +6238,13 @@
       <c r="F53" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="G53" s="108" t="s">
+      <c r="G53" s="107" t="s">
         <v>744</v>
       </c>
       <c r="J53"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A54" s="105" t="s">
+      <c r="A54" s="104" t="s">
         <v>195</v>
       </c>
       <c r="B54" s="75" t="s">
@@ -6259,13 +6260,13 @@
       <c r="F54" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="G54" s="106" t="s">
+      <c r="G54" s="105" t="s">
         <v>745</v>
       </c>
       <c r="J54"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A55" s="107" t="s">
+      <c r="A55" s="106" t="s">
         <v>198</v>
       </c>
       <c r="B55" s="74" t="s">
@@ -6281,13 +6282,13 @@
       <c r="F55" s="72" t="s">
         <v>676</v>
       </c>
-      <c r="G55" s="108" t="s">
+      <c r="G55" s="107" t="s">
         <v>677</v>
       </c>
       <c r="J55"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="104" t="s">
         <v>200</v>
       </c>
       <c r="B56" s="75" t="s">
@@ -6303,13 +6304,13 @@
       <c r="F56" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="G56" s="106" t="s">
+      <c r="G56" s="105" t="s">
         <v>746</v>
       </c>
       <c r="J56"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A57" s="107" t="s">
+      <c r="A57" s="106" t="s">
         <v>204</v>
       </c>
       <c r="B57" s="74" t="s">
@@ -6325,13 +6326,13 @@
       <c r="F57" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="G57" s="108" t="s">
+      <c r="G57" s="107" t="s">
         <v>747</v>
       </c>
       <c r="J57"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A58" s="105" t="s">
+      <c r="A58" s="104" t="s">
         <v>208</v>
       </c>
       <c r="B58" s="75" t="s">
@@ -6347,13 +6348,13 @@
       <c r="F58" s="71" t="s">
         <v>211</v>
       </c>
-      <c r="G58" s="106" t="s">
+      <c r="G58" s="105" t="s">
         <v>61</v>
       </c>
       <c r="J58"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="106" t="s">
         <v>212</v>
       </c>
       <c r="B59" s="74" t="s">
@@ -6369,13 +6370,13 @@
       <c r="F59" s="72" t="s">
         <v>214</v>
       </c>
-      <c r="G59" s="108" t="s">
+      <c r="G59" s="107" t="s">
         <v>748</v>
       </c>
       <c r="J59"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A60" s="105" t="s">
+      <c r="A60" s="104" t="s">
         <v>215</v>
       </c>
       <c r="B60" s="75" t="s">
@@ -6391,13 +6392,13 @@
       <c r="F60" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="G60" s="106" t="s">
+      <c r="G60" s="105" t="s">
         <v>749</v>
       </c>
       <c r="J60"/>
     </row>
     <row r="61" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A61" s="107" t="s">
+      <c r="A61" s="106" t="s">
         <v>219</v>
       </c>
       <c r="B61" s="74" t="s">
@@ -6413,13 +6414,13 @@
       <c r="F61" s="72" t="s">
         <v>679</v>
       </c>
-      <c r="G61" s="108" t="s">
+      <c r="G61" s="107" t="s">
         <v>680</v>
       </c>
       <c r="J61"/>
     </row>
     <row r="62" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A62" s="105" t="s">
+      <c r="A62" s="104" t="s">
         <v>220</v>
       </c>
       <c r="B62" s="75" t="s">
@@ -6435,13 +6436,13 @@
       <c r="F62" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="G62" s="106" t="s">
+      <c r="G62" s="105" t="s">
         <v>750</v>
       </c>
       <c r="J62"/>
     </row>
     <row r="63" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A63" s="107" t="s">
+      <c r="A63" s="106" t="s">
         <v>223</v>
       </c>
       <c r="B63" s="74" t="s">
@@ -6457,13 +6458,13 @@
       <c r="F63" s="72" t="s">
         <v>682</v>
       </c>
-      <c r="G63" s="108" t="s">
+      <c r="G63" s="107" t="s">
         <v>683</v>
       </c>
       <c r="J63"/>
     </row>
     <row r="64" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A64" s="105" t="s">
+      <c r="A64" s="104" t="s">
         <v>226</v>
       </c>
       <c r="B64" s="75" t="s">
@@ -6479,13 +6480,13 @@
       <c r="F64" s="71" t="s">
         <v>229</v>
       </c>
-      <c r="G64" s="106" t="s">
+      <c r="G64" s="105" t="s">
         <v>751</v>
       </c>
       <c r="J64"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A65" s="107" t="s">
+      <c r="A65" s="106" t="s">
         <v>230</v>
       </c>
       <c r="B65" s="74" t="s">
@@ -6501,13 +6502,13 @@
       <c r="F65" s="72" t="s">
         <v>684</v>
       </c>
-      <c r="G65" s="108" t="s">
+      <c r="G65" s="107" t="s">
         <v>685</v>
       </c>
       <c r="J65"/>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A66" s="105" t="s">
+      <c r="A66" s="104" t="s">
         <v>232</v>
       </c>
       <c r="B66" s="75" t="s">
@@ -6523,13 +6524,13 @@
       <c r="F66" s="71" t="s">
         <v>234</v>
       </c>
-      <c r="G66" s="106" t="s">
+      <c r="G66" s="105" t="s">
         <v>94</v>
       </c>
       <c r="J66"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A67" s="107" t="s">
+      <c r="A67" s="106" t="s">
         <v>235</v>
       </c>
       <c r="B67" s="74" t="s">
@@ -6545,13 +6546,13 @@
       <c r="F67" s="72" t="s">
         <v>237</v>
       </c>
-      <c r="G67" s="108" t="s">
+      <c r="G67" s="107" t="s">
         <v>752</v>
       </c>
       <c r="J67"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A68" s="105" t="s">
+      <c r="A68" s="104" t="s">
         <v>238</v>
       </c>
       <c r="B68" s="75" t="s">
@@ -6567,13 +6568,13 @@
       <c r="F68" s="71" t="s">
         <v>240</v>
       </c>
-      <c r="G68" s="106" t="s">
+      <c r="G68" s="105" t="s">
         <v>753</v>
       </c>
       <c r="J68"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A69" s="107" t="s">
+      <c r="A69" s="106" t="s">
         <v>241</v>
       </c>
       <c r="B69" s="74" t="s">
@@ -6589,13 +6590,13 @@
       <c r="F69" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="G69" s="108" t="s">
+      <c r="G69" s="107" t="s">
         <v>754</v>
       </c>
       <c r="J69"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A70" s="105" t="s">
+      <c r="A70" s="104" t="s">
         <v>244</v>
       </c>
       <c r="B70" s="75" t="s">
@@ -6611,13 +6612,13 @@
       <c r="F70" s="71" t="s">
         <v>246</v>
       </c>
-      <c r="G70" s="106" t="s">
+      <c r="G70" s="105" t="s">
         <v>755</v>
       </c>
       <c r="J70"/>
     </row>
     <row r="71" spans="1:10" ht="14.25">
-      <c r="A71" s="107" t="s">
+      <c r="A71" s="106" t="s">
         <v>247</v>
       </c>
       <c r="B71" s="74" t="s">
@@ -6633,13 +6634,13 @@
       <c r="F71" s="72" t="s">
         <v>249</v>
       </c>
-      <c r="G71" s="108" t="s">
+      <c r="G71" s="107" t="s">
         <v>61</v>
       </c>
       <c r="J71"/>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A72" s="105" t="s">
+      <c r="A72" s="104" t="s">
         <v>250</v>
       </c>
       <c r="B72" s="75" t="s">
@@ -6655,13 +6656,13 @@
       <c r="F72" s="71" t="s">
         <v>686</v>
       </c>
-      <c r="G72" s="106" t="s">
+      <c r="G72" s="105" t="s">
         <v>687</v>
       </c>
       <c r="J72"/>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A73" s="107" t="s">
+      <c r="A73" s="106" t="s">
         <v>252</v>
       </c>
       <c r="B73" s="74" t="s">
@@ -6677,13 +6678,13 @@
       <c r="F73" s="72" t="s">
         <v>692</v>
       </c>
-      <c r="G73" s="108" t="s">
+      <c r="G73" s="107" t="s">
         <v>695</v>
       </c>
       <c r="J73"/>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A74" s="105" t="s">
+      <c r="A74" s="104" t="s">
         <v>254</v>
       </c>
       <c r="B74" s="75" t="s">
@@ -6699,13 +6700,13 @@
       <c r="F74" s="71" t="s">
         <v>693</v>
       </c>
-      <c r="G74" s="106" t="s">
+      <c r="G74" s="105" t="s">
         <v>694</v>
       </c>
       <c r="J74"/>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A75" s="107" t="s">
+      <c r="A75" s="106" t="s">
         <v>256</v>
       </c>
       <c r="B75" s="74" t="s">
@@ -6721,35 +6722,35 @@
       <c r="F75" s="72" t="s">
         <v>259</v>
       </c>
-      <c r="G75" s="108"/>
+      <c r="G75" s="107"/>
       <c r="J75"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A76" s="120" t="s">
+      <c r="A76" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="121" t="s">
+      <c r="B76" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="127" t="s">
+      <c r="C76" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="128" t="s">
+      <c r="D76" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="124" t="s">
+      <c r="E76" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="125" t="s">
+      <c r="F76" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="G76" s="126" t="s">
+      <c r="G76" s="125" t="s">
         <v>7</v>
       </c>
       <c r="J76"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A77" s="105" t="s">
+      <c r="A77" s="104" t="s">
         <v>260</v>
       </c>
       <c r="B77" s="75" t="s">
@@ -6765,11 +6766,11 @@
       <c r="F77" s="71" t="s">
         <v>263</v>
       </c>
-      <c r="G77" s="106"/>
+      <c r="G77" s="105"/>
       <c r="J77"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A78" s="107" t="s">
+      <c r="A78" s="106" t="s">
         <v>264</v>
       </c>
       <c r="B78" s="74" t="s">
@@ -6785,13 +6786,13 @@
       <c r="F78" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="G78" s="108" t="s">
+      <c r="G78" s="107" t="s">
         <v>268</v>
       </c>
       <c r="J78"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A79" s="168" t="s">
+      <c r="A79" s="133" t="s">
         <v>269</v>
       </c>
       <c r="B79" s="75" t="s">
@@ -6807,13 +6808,13 @@
       <c r="F79" s="71" t="s">
         <v>697</v>
       </c>
-      <c r="G79" s="106" t="s">
+      <c r="G79" s="105" t="s">
         <v>698</v>
       </c>
       <c r="J79"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A80" s="107" t="s">
+      <c r="A80" s="106" t="s">
         <v>271</v>
       </c>
       <c r="B80" s="74" t="s">
@@ -6829,13 +6830,13 @@
       <c r="F80" s="72" t="s">
         <v>274</v>
       </c>
-      <c r="G80" s="108" t="s">
+      <c r="G80" s="107" t="s">
         <v>756</v>
       </c>
       <c r="J80"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A81" s="105" t="s">
+      <c r="A81" s="104" t="s">
         <v>275</v>
       </c>
       <c r="B81" s="75" t="s">
@@ -6851,13 +6852,13 @@
       <c r="F81" s="71" t="s">
         <v>700</v>
       </c>
-      <c r="G81" s="106" t="s">
+      <c r="G81" s="105" t="s">
         <v>699</v>
       </c>
       <c r="J81"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A82" s="107" t="s">
+      <c r="A82" s="106" t="s">
         <v>278</v>
       </c>
       <c r="B82" s="74" t="s">
@@ -6873,13 +6874,13 @@
       <c r="F82" s="72" t="s">
         <v>280</v>
       </c>
-      <c r="G82" s="108" t="s">
+      <c r="G82" s="107" t="s">
         <v>757</v>
       </c>
       <c r="J82"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A83" s="105" t="s">
+      <c r="A83" s="104" t="s">
         <v>281</v>
       </c>
       <c r="B83" s="75" t="s">
@@ -6895,13 +6896,13 @@
       <c r="F83" s="71" t="s">
         <v>703</v>
       </c>
-      <c r="G83" s="106" t="s">
+      <c r="G83" s="105" t="s">
         <v>704</v>
       </c>
       <c r="J83"/>
     </row>
     <row r="84" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A84" s="107" t="s">
+      <c r="A84" s="106" t="s">
         <v>284</v>
       </c>
       <c r="B84" s="74" t="s">
@@ -6917,13 +6918,13 @@
       <c r="F84" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="G84" s="108" t="s">
+      <c r="G84" s="107" t="s">
         <v>758</v>
       </c>
       <c r="J84"/>
     </row>
     <row r="85" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A85" s="168" t="s">
+      <c r="A85" s="133" t="s">
         <v>287</v>
       </c>
       <c r="B85" s="75" t="s">
@@ -6939,13 +6940,13 @@
       <c r="F85" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="G85" s="106" t="s">
+      <c r="G85" s="105" t="s">
         <v>759</v>
       </c>
       <c r="J85"/>
     </row>
     <row r="86" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A86" s="107" t="s">
+      <c r="A86" s="106" t="s">
         <v>290</v>
       </c>
       <c r="B86" s="74" t="s">
@@ -6961,13 +6962,13 @@
       <c r="F86" s="72" t="s">
         <v>702</v>
       </c>
-      <c r="G86" s="108" t="s">
+      <c r="G86" s="107" t="s">
         <v>701</v>
       </c>
       <c r="J86"/>
     </row>
     <row r="87" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A87" s="105" t="s">
+      <c r="A87" s="104" t="s">
         <v>293</v>
       </c>
       <c r="B87" s="75" t="s">
@@ -6983,13 +6984,13 @@
       <c r="F87" s="71" t="s">
         <v>296</v>
       </c>
-      <c r="G87" s="106" t="s">
+      <c r="G87" s="105" t="s">
         <v>760</v>
       </c>
       <c r="J87"/>
     </row>
     <row r="88" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A88" s="107" t="s">
+      <c r="A88" s="106" t="s">
         <v>297</v>
       </c>
       <c r="B88" s="93" t="s">
@@ -7005,13 +7006,13 @@
       <c r="F88" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="G88" s="108" t="s">
+      <c r="G88" s="107" t="s">
         <v>761</v>
       </c>
       <c r="J88"/>
     </row>
     <row r="89" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A89" s="105" t="s">
+      <c r="A89" s="104" t="s">
         <v>300</v>
       </c>
       <c r="B89" s="75" t="s">
@@ -7027,13 +7028,13 @@
       <c r="F89" s="71" t="s">
         <v>302</v>
       </c>
-      <c r="G89" s="106" t="s">
+      <c r="G89" s="105" t="s">
         <v>762</v>
       </c>
       <c r="J89"/>
     </row>
     <row r="90" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A90" s="107" t="s">
+      <c r="A90" s="106" t="s">
         <v>303</v>
       </c>
       <c r="B90" s="74" t="s">
@@ -7049,13 +7050,13 @@
       <c r="F90" s="72" t="s">
         <v>306</v>
       </c>
-      <c r="G90" s="108" t="s">
+      <c r="G90" s="107" t="s">
         <v>763</v>
       </c>
       <c r="J90"/>
     </row>
     <row r="91" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A91" s="105" t="s">
+      <c r="A91" s="104" t="s">
         <v>307</v>
       </c>
       <c r="B91" s="75" t="s">
@@ -7071,13 +7072,13 @@
       <c r="F91" s="71" t="s">
         <v>309</v>
       </c>
-      <c r="G91" s="106" t="s">
+      <c r="G91" s="105" t="s">
         <v>648</v>
       </c>
       <c r="J91"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A92" s="107" t="s">
+      <c r="A92" s="106" t="s">
         <v>310</v>
       </c>
       <c r="B92" s="74" t="s">
@@ -7093,13 +7094,13 @@
       <c r="F92" s="72" t="s">
         <v>312</v>
       </c>
-      <c r="G92" s="108" t="s">
+      <c r="G92" s="107" t="s">
         <v>764</v>
       </c>
       <c r="J92"/>
     </row>
     <row r="93" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A93" s="105" t="s">
+      <c r="A93" s="104" t="s">
         <v>313</v>
       </c>
       <c r="B93" s="75" t="s">
@@ -7115,13 +7116,13 @@
       <c r="F93" s="71" t="s">
         <v>314</v>
       </c>
-      <c r="G93" s="106" t="s">
+      <c r="G93" s="105" t="s">
         <v>765</v>
       </c>
       <c r="J93"/>
     </row>
     <row r="94" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A94" s="107" t="s">
+      <c r="A94" s="106" t="s">
         <v>315</v>
       </c>
       <c r="B94" s="74" t="s">
@@ -7137,13 +7138,13 @@
       <c r="F94" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="G94" s="108" t="s">
+      <c r="G94" s="107" t="s">
         <v>766</v>
       </c>
       <c r="J94"/>
     </row>
     <row r="95" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A95" s="105" t="s">
+      <c r="A95" s="104" t="s">
         <v>319</v>
       </c>
       <c r="B95" s="95" t="s">
@@ -7159,13 +7160,13 @@
       <c r="F95" s="71" t="s">
         <v>322</v>
       </c>
-      <c r="G95" s="106" t="s">
+      <c r="G95" s="105" t="s">
         <v>767</v>
       </c>
       <c r="J95"/>
     </row>
     <row r="96" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A96" s="107" t="s">
+      <c r="A96" s="106" t="s">
         <v>323</v>
       </c>
       <c r="B96" s="74" t="s">
@@ -7181,13 +7182,13 @@
       <c r="F96" s="72" t="s">
         <v>326</v>
       </c>
-      <c r="G96" s="108" t="s">
+      <c r="G96" s="107" t="s">
         <v>769</v>
       </c>
       <c r="J96"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A97" s="105" t="s">
+      <c r="A97" s="104" t="s">
         <v>327</v>
       </c>
       <c r="B97" s="75" t="s">
@@ -7203,13 +7204,13 @@
       <c r="F97" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="G97" s="106" t="s">
+      <c r="G97" s="105" t="s">
         <v>768</v>
       </c>
       <c r="J97"/>
     </row>
     <row r="98" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A98" s="107" t="s">
+      <c r="A98" s="106" t="s">
         <v>331</v>
       </c>
       <c r="B98" s="74" t="s">
@@ -7225,13 +7226,13 @@
       <c r="F98" s="72" t="s">
         <v>333</v>
       </c>
-      <c r="G98" s="108" t="s">
+      <c r="G98" s="107" t="s">
         <v>334</v>
       </c>
       <c r="J98"/>
     </row>
     <row r="99" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A99" s="105" t="s">
+      <c r="A99" s="104" t="s">
         <v>335</v>
       </c>
       <c r="B99" s="75" t="s">
@@ -7247,13 +7248,13 @@
       <c r="F99" s="71" t="s">
         <v>337</v>
       </c>
-      <c r="G99" s="106" t="s">
+      <c r="G99" s="105" t="s">
         <v>338</v>
       </c>
       <c r="J99"/>
     </row>
     <row r="100" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A100" s="107" t="s">
+      <c r="A100" s="106" t="s">
         <v>339</v>
       </c>
       <c r="B100" s="74" t="s">
@@ -7269,13 +7270,13 @@
       <c r="F100" s="72" t="s">
         <v>342</v>
       </c>
-      <c r="G100" s="108" t="s">
+      <c r="G100" s="107" t="s">
         <v>343</v>
       </c>
       <c r="J100"/>
     </row>
     <row r="101" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A101" s="105" t="s">
+      <c r="A101" s="104" t="s">
         <v>344</v>
       </c>
       <c r="B101" s="75" t="s">
@@ -7291,13 +7292,13 @@
       <c r="F101" s="71" t="s">
         <v>346</v>
       </c>
-      <c r="G101" s="106" t="s">
+      <c r="G101" s="105" t="s">
         <v>347</v>
       </c>
       <c r="J101"/>
     </row>
     <row r="102" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A102" s="107" t="s">
+      <c r="A102" s="106" t="s">
         <v>348</v>
       </c>
       <c r="B102" s="74" t="s">
@@ -7313,13 +7314,13 @@
       <c r="F102" s="72" t="s">
         <v>351</v>
       </c>
-      <c r="G102" s="108" t="s">
+      <c r="G102" s="107" t="s">
         <v>352</v>
       </c>
       <c r="J102"/>
     </row>
     <row r="103" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A103" s="105" t="s">
+      <c r="A103" s="104" t="s">
         <v>353</v>
       </c>
       <c r="B103" s="75" t="s">
@@ -7335,13 +7336,13 @@
       <c r="F103" s="71" t="s">
         <v>356</v>
       </c>
-      <c r="G103" s="106" t="s">
+      <c r="G103" s="105" t="s">
         <v>357</v>
       </c>
       <c r="J103"/>
     </row>
     <row r="104" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A104" s="107" t="s">
+      <c r="A104" s="106" t="s">
         <v>358</v>
       </c>
       <c r="B104" s="74" t="s">
@@ -7357,13 +7358,13 @@
       <c r="F104" s="72" t="s">
         <v>361</v>
       </c>
-      <c r="G104" s="108" t="s">
+      <c r="G104" s="107" t="s">
         <v>174</v>
       </c>
       <c r="J104"/>
     </row>
     <row r="105" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A105" s="107" t="s">
+      <c r="A105" s="106" t="s">
         <v>362</v>
       </c>
       <c r="B105" s="93"/>
@@ -7371,11 +7372,11 @@
       <c r="D105" s="97"/>
       <c r="E105" s="94"/>
       <c r="F105" s="72"/>
-      <c r="G105" s="111"/>
+      <c r="G105" s="110"/>
       <c r="J105"/>
     </row>
     <row r="106" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A106" s="107" t="s">
+      <c r="A106" s="106" t="s">
         <v>363</v>
       </c>
       <c r="B106" s="74"/>
@@ -7383,11 +7384,11 @@
       <c r="D106" s="85"/>
       <c r="E106" s="86"/>
       <c r="F106" s="72"/>
-      <c r="G106" s="108"/>
+      <c r="G106" s="107"/>
       <c r="J106"/>
     </row>
     <row r="107" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A107" s="107" t="s">
+      <c r="A107" s="106" t="s">
         <v>364</v>
       </c>
       <c r="B107" s="93"/>
@@ -7395,11 +7396,11 @@
       <c r="D107" s="97"/>
       <c r="E107" s="94"/>
       <c r="F107" s="72"/>
-      <c r="G107" s="111"/>
+      <c r="G107" s="110"/>
       <c r="J107"/>
     </row>
     <row r="108" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A108" s="107" t="s">
+      <c r="A108" s="106" t="s">
         <v>365</v>
       </c>
       <c r="B108" s="74"/>
@@ -7407,11 +7408,11 @@
       <c r="D108" s="85"/>
       <c r="E108" s="86"/>
       <c r="F108" s="72"/>
-      <c r="G108" s="108"/>
+      <c r="G108" s="107"/>
       <c r="J108"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A109" s="107" t="s">
+      <c r="A109" s="106" t="s">
         <v>366</v>
       </c>
       <c r="B109" s="93"/>
@@ -7419,11 +7420,11 @@
       <c r="D109" s="97"/>
       <c r="E109" s="94"/>
       <c r="F109" s="72"/>
-      <c r="G109" s="111"/>
+      <c r="G109" s="110"/>
       <c r="J109"/>
     </row>
     <row r="110" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A110" s="107" t="s">
+      <c r="A110" s="106" t="s">
         <v>367</v>
       </c>
       <c r="B110" s="74"/>
@@ -7431,11 +7432,11 @@
       <c r="D110" s="85"/>
       <c r="E110" s="86"/>
       <c r="F110" s="72"/>
-      <c r="G110" s="108"/>
+      <c r="G110" s="107"/>
       <c r="J110"/>
     </row>
     <row r="111" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A111" s="107" t="s">
+      <c r="A111" s="106" t="s">
         <v>368</v>
       </c>
       <c r="B111" s="93"/>
@@ -7443,11 +7444,11 @@
       <c r="D111" s="97"/>
       <c r="E111" s="94"/>
       <c r="F111" s="72"/>
-      <c r="G111" s="111"/>
+      <c r="G111" s="110"/>
       <c r="J111"/>
     </row>
     <row r="112" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A112" s="107" t="s">
+      <c r="A112" s="106" t="s">
         <v>369</v>
       </c>
       <c r="B112" s="74"/>
@@ -7455,11 +7456,11 @@
       <c r="D112" s="85"/>
       <c r="E112" s="86"/>
       <c r="F112" s="72"/>
-      <c r="G112" s="108"/>
+      <c r="G112" s="107"/>
       <c r="J112"/>
     </row>
     <row r="113" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A113" s="107" t="s">
+      <c r="A113" s="106" t="s">
         <v>370</v>
       </c>
       <c r="B113" s="93"/>
@@ -7467,11 +7468,11 @@
       <c r="D113" s="97"/>
       <c r="E113" s="94"/>
       <c r="F113" s="72"/>
-      <c r="G113" s="111"/>
+      <c r="G113" s="110"/>
       <c r="J113"/>
     </row>
     <row r="114" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A114" s="107" t="s">
+      <c r="A114" s="106" t="s">
         <v>371</v>
       </c>
       <c r="B114" s="74"/>
@@ -7479,11 +7480,11 @@
       <c r="D114" s="85"/>
       <c r="E114" s="86"/>
       <c r="F114" s="72"/>
-      <c r="G114" s="108"/>
+      <c r="G114" s="107"/>
       <c r="J114"/>
     </row>
     <row r="115" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A115" s="107" t="s">
+      <c r="A115" s="106" t="s">
         <v>372</v>
       </c>
       <c r="B115" s="93"/>
@@ -7491,11 +7492,11 @@
       <c r="D115" s="97"/>
       <c r="E115" s="94"/>
       <c r="F115" s="72"/>
-      <c r="G115" s="111"/>
+      <c r="G115" s="110"/>
       <c r="J115"/>
     </row>
     <row r="116" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A116" s="107" t="s">
+      <c r="A116" s="106" t="s">
         <v>373</v>
       </c>
       <c r="B116" s="74"/>
@@ -7503,11 +7504,11 @@
       <c r="D116" s="85"/>
       <c r="E116" s="86"/>
       <c r="F116" s="72"/>
-      <c r="G116" s="108"/>
+      <c r="G116" s="107"/>
       <c r="J116"/>
     </row>
     <row r="117" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A117" s="107" t="s">
+      <c r="A117" s="106" t="s">
         <v>374</v>
       </c>
       <c r="B117" s="93"/>
@@ -7515,11 +7516,11 @@
       <c r="D117" s="97"/>
       <c r="E117" s="94"/>
       <c r="F117" s="72"/>
-      <c r="G117" s="111"/>
+      <c r="G117" s="110"/>
       <c r="J117"/>
     </row>
     <row r="118" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A118" s="107" t="s">
+      <c r="A118" s="106" t="s">
         <v>375</v>
       </c>
       <c r="B118" s="74"/>
@@ -7527,11 +7528,11 @@
       <c r="D118" s="85"/>
       <c r="E118" s="86"/>
       <c r="F118" s="72"/>
-      <c r="G118" s="108"/>
+      <c r="G118" s="107"/>
       <c r="J118"/>
     </row>
     <row r="119" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A119" s="107" t="s">
+      <c r="A119" s="106" t="s">
         <v>376</v>
       </c>
       <c r="B119" s="93"/>
@@ -7539,11 +7540,11 @@
       <c r="D119" s="97"/>
       <c r="E119" s="94"/>
       <c r="F119" s="72"/>
-      <c r="G119" s="111"/>
+      <c r="G119" s="110"/>
       <c r="J119"/>
     </row>
     <row r="120" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A120" s="107" t="s">
+      <c r="A120" s="106" t="s">
         <v>377</v>
       </c>
       <c r="B120" s="74"/>
@@ -7551,11 +7552,11 @@
       <c r="D120" s="85"/>
       <c r="E120" s="86"/>
       <c r="F120" s="72"/>
-      <c r="G120" s="108"/>
+      <c r="G120" s="107"/>
       <c r="J120"/>
     </row>
     <row r="121" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A121" s="107" t="s">
+      <c r="A121" s="106" t="s">
         <v>378</v>
       </c>
       <c r="B121" s="93"/>
@@ -7563,11 +7564,11 @@
       <c r="D121" s="97"/>
       <c r="E121" s="94"/>
       <c r="F121" s="72"/>
-      <c r="G121" s="111"/>
+      <c r="G121" s="110"/>
       <c r="J121"/>
     </row>
     <row r="122" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A122" s="107" t="s">
+      <c r="A122" s="106" t="s">
         <v>379</v>
       </c>
       <c r="B122" s="74"/>
@@ -7575,11 +7576,11 @@
       <c r="D122" s="85"/>
       <c r="E122" s="86"/>
       <c r="F122" s="72"/>
-      <c r="G122" s="108"/>
+      <c r="G122" s="107"/>
       <c r="J122"/>
     </row>
     <row r="123" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A123" s="107" t="s">
+      <c r="A123" s="106" t="s">
         <v>380</v>
       </c>
       <c r="B123" s="93"/>
@@ -7587,11 +7588,11 @@
       <c r="D123" s="97"/>
       <c r="E123" s="94"/>
       <c r="F123" s="72"/>
-      <c r="G123" s="111"/>
+      <c r="G123" s="110"/>
       <c r="J123"/>
     </row>
     <row r="124" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A124" s="107" t="s">
+      <c r="A124" s="106" t="s">
         <v>381</v>
       </c>
       <c r="B124" s="74"/>
@@ -7599,11 +7600,11 @@
       <c r="D124" s="85"/>
       <c r="E124" s="86"/>
       <c r="F124" s="72"/>
-      <c r="G124" s="108"/>
+      <c r="G124" s="107"/>
       <c r="J124"/>
     </row>
     <row r="125" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A125" s="107" t="s">
+      <c r="A125" s="106" t="s">
         <v>382</v>
       </c>
       <c r="B125" s="93"/>
@@ -7611,11 +7612,11 @@
       <c r="D125" s="97"/>
       <c r="E125" s="94"/>
       <c r="F125" s="72"/>
-      <c r="G125" s="111"/>
+      <c r="G125" s="110"/>
       <c r="J125"/>
     </row>
     <row r="126" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A126" s="107" t="s">
+      <c r="A126" s="106" t="s">
         <v>383</v>
       </c>
       <c r="B126" s="74"/>
@@ -7623,11 +7624,11 @@
       <c r="D126" s="85"/>
       <c r="E126" s="86"/>
       <c r="F126" s="72"/>
-      <c r="G126" s="108"/>
+      <c r="G126" s="107"/>
       <c r="J126"/>
     </row>
     <row r="127" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A127" s="107" t="s">
+      <c r="A127" s="106" t="s">
         <v>384</v>
       </c>
       <c r="B127" s="93"/>
@@ -7635,11 +7636,11 @@
       <c r="D127" s="97"/>
       <c r="E127" s="94"/>
       <c r="F127" s="72"/>
-      <c r="G127" s="111"/>
+      <c r="G127" s="110"/>
       <c r="J127"/>
     </row>
     <row r="128" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A128" s="107" t="s">
+      <c r="A128" s="106" t="s">
         <v>385</v>
       </c>
       <c r="B128" s="74"/>
@@ -7647,11 +7648,11 @@
       <c r="D128" s="85"/>
       <c r="E128" s="86"/>
       <c r="F128" s="72"/>
-      <c r="G128" s="108"/>
+      <c r="G128" s="107"/>
       <c r="J128"/>
     </row>
     <row r="129" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A129" s="107" t="s">
+      <c r="A129" s="106" t="s">
         <v>386</v>
       </c>
       <c r="B129" s="93"/>
@@ -7659,11 +7660,11 @@
       <c r="D129" s="97"/>
       <c r="E129" s="94"/>
       <c r="F129" s="72"/>
-      <c r="G129" s="111"/>
+      <c r="G129" s="110"/>
       <c r="J129"/>
     </row>
     <row r="130" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A130" s="107" t="s">
+      <c r="A130" s="106" t="s">
         <v>387</v>
       </c>
       <c r="B130" s="74"/>
@@ -7671,11 +7672,11 @@
       <c r="D130" s="85"/>
       <c r="E130" s="86"/>
       <c r="F130" s="72"/>
-      <c r="G130" s="108"/>
+      <c r="G130" s="107"/>
       <c r="J130"/>
     </row>
     <row r="131" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A131" s="107" t="s">
+      <c r="A131" s="106" t="s">
         <v>388</v>
       </c>
       <c r="B131" s="93"/>
@@ -7683,11 +7684,11 @@
       <c r="D131" s="97"/>
       <c r="E131" s="94"/>
       <c r="F131" s="72"/>
-      <c r="G131" s="111"/>
+      <c r="G131" s="110"/>
       <c r="J131"/>
     </row>
     <row r="132" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A132" s="107" t="s">
+      <c r="A132" s="106" t="s">
         <v>389</v>
       </c>
       <c r="B132" s="74"/>
@@ -7695,11 +7696,11 @@
       <c r="D132" s="85"/>
       <c r="E132" s="86"/>
       <c r="F132" s="72"/>
-      <c r="G132" s="108"/>
+      <c r="G132" s="107"/>
       <c r="J132"/>
     </row>
     <row r="133" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A133" s="107" t="s">
+      <c r="A133" s="106" t="s">
         <v>390</v>
       </c>
       <c r="B133" s="93"/>
@@ -7707,11 +7708,11 @@
       <c r="D133" s="97"/>
       <c r="E133" s="94"/>
       <c r="F133" s="72"/>
-      <c r="G133" s="111"/>
+      <c r="G133" s="110"/>
       <c r="J133"/>
     </row>
     <row r="134" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A134" s="107" t="s">
+      <c r="A134" s="106" t="s">
         <v>391</v>
       </c>
       <c r="B134" s="74"/>
@@ -7719,11 +7720,11 @@
       <c r="D134" s="85"/>
       <c r="E134" s="86"/>
       <c r="F134" s="72"/>
-      <c r="G134" s="108"/>
+      <c r="G134" s="107"/>
       <c r="J134"/>
     </row>
     <row r="135" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A135" s="107" t="s">
+      <c r="A135" s="106" t="s">
         <v>392</v>
       </c>
       <c r="B135" s="93"/>
@@ -7731,11 +7732,11 @@
       <c r="D135" s="97"/>
       <c r="E135" s="94"/>
       <c r="F135" s="72"/>
-      <c r="G135" s="111"/>
+      <c r="G135" s="110"/>
       <c r="J135"/>
     </row>
     <row r="136" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A136" s="107" t="s">
+      <c r="A136" s="106" t="s">
         <v>393</v>
       </c>
       <c r="B136" s="74"/>
@@ -7743,11 +7744,11 @@
       <c r="D136" s="85"/>
       <c r="E136" s="86"/>
       <c r="F136" s="72"/>
-      <c r="G136" s="108"/>
+      <c r="G136" s="107"/>
       <c r="J136"/>
     </row>
     <row r="137" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A137" s="107" t="s">
+      <c r="A137" s="106" t="s">
         <v>394</v>
       </c>
       <c r="B137" s="93"/>
@@ -7755,11 +7756,11 @@
       <c r="D137" s="97"/>
       <c r="E137" s="94"/>
       <c r="F137" s="72"/>
-      <c r="G137" s="111"/>
+      <c r="G137" s="110"/>
       <c r="J137"/>
     </row>
     <row r="138" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A138" s="107" t="s">
+      <c r="A138" s="106" t="s">
         <v>395</v>
       </c>
       <c r="B138" s="74"/>
@@ -7767,11 +7768,11 @@
       <c r="D138" s="85"/>
       <c r="E138" s="86"/>
       <c r="F138" s="72"/>
-      <c r="G138" s="108"/>
+      <c r="G138" s="107"/>
       <c r="J138"/>
     </row>
     <row r="139" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A139" s="107" t="s">
+      <c r="A139" s="106" t="s">
         <v>396</v>
       </c>
       <c r="B139" s="93"/>
@@ -7779,11 +7780,11 @@
       <c r="D139" s="97"/>
       <c r="E139" s="94"/>
       <c r="F139" s="72"/>
-      <c r="G139" s="111"/>
+      <c r="G139" s="110"/>
       <c r="J139"/>
     </row>
     <row r="140" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A140" s="107" t="s">
+      <c r="A140" s="106" t="s">
         <v>397</v>
       </c>
       <c r="B140" s="74"/>
@@ -7791,11 +7792,11 @@
       <c r="D140" s="85"/>
       <c r="E140" s="86"/>
       <c r="F140" s="72"/>
-      <c r="G140" s="108"/>
+      <c r="G140" s="107"/>
       <c r="J140"/>
     </row>
     <row r="141" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A141" s="107" t="s">
+      <c r="A141" s="106" t="s">
         <v>398</v>
       </c>
       <c r="B141" s="93"/>
@@ -7803,11 +7804,11 @@
       <c r="D141" s="97"/>
       <c r="E141" s="94"/>
       <c r="F141" s="72"/>
-      <c r="G141" s="111"/>
+      <c r="G141" s="110"/>
       <c r="J141"/>
     </row>
     <row r="142" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A142" s="107" t="s">
+      <c r="A142" s="106" t="s">
         <v>399</v>
       </c>
       <c r="B142" s="74"/>
@@ -7815,11 +7816,11 @@
       <c r="D142" s="85"/>
       <c r="E142" s="86"/>
       <c r="F142" s="72"/>
-      <c r="G142" s="108"/>
+      <c r="G142" s="107"/>
       <c r="J142"/>
     </row>
     <row r="143" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A143" s="107" t="s">
+      <c r="A143" s="106" t="s">
         <v>400</v>
       </c>
       <c r="B143" s="93"/>
@@ -7827,11 +7828,11 @@
       <c r="D143" s="97"/>
       <c r="E143" s="94"/>
       <c r="F143" s="72"/>
-      <c r="G143" s="111"/>
+      <c r="G143" s="110"/>
       <c r="J143"/>
     </row>
     <row r="144" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A144" s="107" t="s">
+      <c r="A144" s="106" t="s">
         <v>401</v>
       </c>
       <c r="B144" s="74"/>
@@ -7839,11 +7840,11 @@
       <c r="D144" s="85"/>
       <c r="E144" s="86"/>
       <c r="F144" s="72"/>
-      <c r="G144" s="108"/>
+      <c r="G144" s="107"/>
       <c r="J144"/>
     </row>
     <row r="145" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A145" s="107" t="s">
+      <c r="A145" s="106" t="s">
         <v>402</v>
       </c>
       <c r="B145" s="93"/>
@@ -7851,11 +7852,11 @@
       <c r="D145" s="97"/>
       <c r="E145" s="94"/>
       <c r="F145" s="72"/>
-      <c r="G145" s="111"/>
+      <c r="G145" s="110"/>
       <c r="J145"/>
     </row>
     <row r="146" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A146" s="107" t="s">
+      <c r="A146" s="106" t="s">
         <v>403</v>
       </c>
       <c r="B146" s="74"/>
@@ -7863,11 +7864,11 @@
       <c r="D146" s="85"/>
       <c r="E146" s="86"/>
       <c r="F146" s="72"/>
-      <c r="G146" s="108"/>
+      <c r="G146" s="107"/>
       <c r="J146"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A147" s="107" t="s">
+      <c r="A147" s="106" t="s">
         <v>404</v>
       </c>
       <c r="B147" s="93"/>
@@ -7875,11 +7876,11 @@
       <c r="D147" s="97"/>
       <c r="E147" s="94"/>
       <c r="F147" s="72"/>
-      <c r="G147" s="111"/>
+      <c r="G147" s="110"/>
       <c r="J147"/>
     </row>
     <row r="148" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A148" s="107" t="s">
+      <c r="A148" s="106" t="s">
         <v>405</v>
       </c>
       <c r="B148" s="74"/>
@@ -7887,11 +7888,11 @@
       <c r="D148" s="85"/>
       <c r="E148" s="86"/>
       <c r="F148" s="72"/>
-      <c r="G148" s="108"/>
+      <c r="G148" s="107"/>
       <c r="J148"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A149" s="107" t="s">
+      <c r="A149" s="106" t="s">
         <v>406</v>
       </c>
       <c r="B149" s="93"/>
@@ -7899,11 +7900,11 @@
       <c r="D149" s="97"/>
       <c r="E149" s="94"/>
       <c r="F149" s="72"/>
-      <c r="G149" s="111"/>
+      <c r="G149" s="110"/>
       <c r="J149"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A150" s="107" t="s">
+      <c r="A150" s="106" t="s">
         <v>407</v>
       </c>
       <c r="B150" s="74"/>
@@ -7911,11 +7912,11 @@
       <c r="D150" s="85"/>
       <c r="E150" s="86"/>
       <c r="F150" s="72"/>
-      <c r="G150" s="108"/>
+      <c r="G150" s="107"/>
       <c r="J150"/>
     </row>
     <row r="151" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A151" s="107" t="s">
+      <c r="A151" s="106" t="s">
         <v>408</v>
       </c>
       <c r="B151" s="93"/>
@@ -7923,11 +7924,11 @@
       <c r="D151" s="97"/>
       <c r="E151" s="94"/>
       <c r="F151" s="72"/>
-      <c r="G151" s="111"/>
+      <c r="G151" s="110"/>
       <c r="J151"/>
     </row>
     <row r="152" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A152" s="107" t="s">
+      <c r="A152" s="106" t="s">
         <v>409</v>
       </c>
       <c r="B152" s="74"/>
@@ -7935,11 +7936,11 @@
       <c r="D152" s="85"/>
       <c r="E152" s="86"/>
       <c r="F152" s="72"/>
-      <c r="G152" s="108"/>
+      <c r="G152" s="107"/>
       <c r="J152"/>
     </row>
     <row r="153" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A153" s="107" t="s">
+      <c r="A153" s="106" t="s">
         <v>410</v>
       </c>
       <c r="B153" s="93"/>
@@ -7947,11 +7948,11 @@
       <c r="D153" s="97"/>
       <c r="E153" s="94"/>
       <c r="F153" s="72"/>
-      <c r="G153" s="111"/>
+      <c r="G153" s="110"/>
       <c r="J153"/>
     </row>
     <row r="154" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A154" s="107" t="s">
+      <c r="A154" s="106" t="s">
         <v>411</v>
       </c>
       <c r="B154" s="74"/>
@@ -7959,11 +7960,11 @@
       <c r="D154" s="85"/>
       <c r="E154" s="86"/>
       <c r="F154" s="72"/>
-      <c r="G154" s="108"/>
+      <c r="G154" s="107"/>
       <c r="J154"/>
     </row>
     <row r="155" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A155" s="107" t="s">
+      <c r="A155" s="106" t="s">
         <v>412</v>
       </c>
       <c r="B155" s="93"/>
@@ -7971,11 +7972,11 @@
       <c r="D155" s="97"/>
       <c r="E155" s="94"/>
       <c r="F155" s="72"/>
-      <c r="G155" s="111"/>
+      <c r="G155" s="110"/>
       <c r="J155"/>
     </row>
     <row r="156" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A156" s="107" t="s">
+      <c r="A156" s="106" t="s">
         <v>413</v>
       </c>
       <c r="B156" s="74"/>
@@ -7983,11 +7984,11 @@
       <c r="D156" s="85"/>
       <c r="E156" s="86"/>
       <c r="F156" s="72"/>
-      <c r="G156" s="108"/>
+      <c r="G156" s="107"/>
       <c r="J156"/>
     </row>
     <row r="157" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A157" s="107" t="s">
+      <c r="A157" s="106" t="s">
         <v>414</v>
       </c>
       <c r="B157" s="93"/>
@@ -7995,11 +7996,11 @@
       <c r="D157" s="97"/>
       <c r="E157" s="94"/>
       <c r="F157" s="72"/>
-      <c r="G157" s="111"/>
+      <c r="G157" s="110"/>
       <c r="J157"/>
     </row>
     <row r="158" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A158" s="107" t="s">
+      <c r="A158" s="106" t="s">
         <v>415</v>
       </c>
       <c r="B158" s="74"/>
@@ -8007,11 +8008,11 @@
       <c r="D158" s="85"/>
       <c r="E158" s="86"/>
       <c r="F158" s="72"/>
-      <c r="G158" s="108"/>
+      <c r="G158" s="107"/>
       <c r="J158"/>
     </row>
     <row r="159" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A159" s="107" t="s">
+      <c r="A159" s="106" t="s">
         <v>416</v>
       </c>
       <c r="B159" s="93"/>
@@ -8019,11 +8020,11 @@
       <c r="D159" s="97"/>
       <c r="E159" s="94"/>
       <c r="F159" s="72"/>
-      <c r="G159" s="111"/>
+      <c r="G159" s="110"/>
       <c r="J159"/>
     </row>
     <row r="160" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A160" s="107" t="s">
+      <c r="A160" s="106" t="s">
         <v>417</v>
       </c>
       <c r="B160" s="74"/>
@@ -8031,11 +8032,11 @@
       <c r="D160" s="85"/>
       <c r="E160" s="86"/>
       <c r="F160" s="72"/>
-      <c r="G160" s="108"/>
+      <c r="G160" s="107"/>
       <c r="J160"/>
     </row>
     <row r="161" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A161" s="107" t="s">
+      <c r="A161" s="106" t="s">
         <v>418</v>
       </c>
       <c r="B161" s="93"/>
@@ -8043,11 +8044,11 @@
       <c r="D161" s="97"/>
       <c r="E161" s="94"/>
       <c r="F161" s="72"/>
-      <c r="G161" s="111"/>
+      <c r="G161" s="110"/>
       <c r="J161"/>
     </row>
     <row r="162" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A162" s="107" t="s">
+      <c r="A162" s="106" t="s">
         <v>419</v>
       </c>
       <c r="B162" s="74"/>
@@ -8055,11 +8056,11 @@
       <c r="D162" s="85"/>
       <c r="E162" s="86"/>
       <c r="F162" s="72"/>
-      <c r="G162" s="108"/>
+      <c r="G162" s="107"/>
       <c r="J162"/>
     </row>
     <row r="163" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A163" s="107" t="s">
+      <c r="A163" s="106" t="s">
         <v>420</v>
       </c>
       <c r="B163" s="93"/>
@@ -8067,11 +8068,11 @@
       <c r="D163" s="97"/>
       <c r="E163" s="94"/>
       <c r="F163" s="72"/>
-      <c r="G163" s="111"/>
+      <c r="G163" s="110"/>
       <c r="J163"/>
     </row>
     <row r="164" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A164" s="107" t="s">
+      <c r="A164" s="106" t="s">
         <v>421</v>
       </c>
       <c r="B164" s="74"/>
@@ -8079,11 +8080,11 @@
       <c r="D164" s="85"/>
       <c r="E164" s="86"/>
       <c r="F164" s="72"/>
-      <c r="G164" s="108"/>
+      <c r="G164" s="107"/>
       <c r="J164"/>
     </row>
     <row r="165" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A165" s="107" t="s">
+      <c r="A165" s="106" t="s">
         <v>422</v>
       </c>
       <c r="B165" s="93"/>
@@ -8091,11 +8092,11 @@
       <c r="D165" s="97"/>
       <c r="E165" s="94"/>
       <c r="F165" s="72"/>
-      <c r="G165" s="111"/>
+      <c r="G165" s="110"/>
       <c r="J165"/>
     </row>
     <row r="166" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A166" s="107" t="s">
+      <c r="A166" s="106" t="s">
         <v>423</v>
       </c>
       <c r="B166" s="74"/>
@@ -8103,11 +8104,11 @@
       <c r="D166" s="85"/>
       <c r="E166" s="86"/>
       <c r="F166" s="72"/>
-      <c r="G166" s="108"/>
+      <c r="G166" s="107"/>
       <c r="J166"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A167" s="107" t="s">
+      <c r="A167" s="106" t="s">
         <v>424</v>
       </c>
       <c r="B167" s="93"/>
@@ -8115,11 +8116,11 @@
       <c r="D167" s="97"/>
       <c r="E167" s="94"/>
       <c r="F167" s="72"/>
-      <c r="G167" s="111"/>
+      <c r="G167" s="110"/>
       <c r="J167"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A168" s="107" t="s">
+      <c r="A168" s="106" t="s">
         <v>425</v>
       </c>
       <c r="B168" s="74"/>
@@ -8127,11 +8128,11 @@
       <c r="D168" s="85"/>
       <c r="E168" s="86"/>
       <c r="F168" s="72"/>
-      <c r="G168" s="108"/>
+      <c r="G168" s="107"/>
       <c r="J168"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A169" s="107" t="s">
+      <c r="A169" s="106" t="s">
         <v>426</v>
       </c>
       <c r="B169" s="93"/>
@@ -8139,11 +8140,11 @@
       <c r="D169" s="97"/>
       <c r="E169" s="94"/>
       <c r="F169" s="72"/>
-      <c r="G169" s="111"/>
+      <c r="G169" s="110"/>
       <c r="J169"/>
     </row>
     <row r="170" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A170" s="107" t="s">
+      <c r="A170" s="106" t="s">
         <v>427</v>
       </c>
       <c r="B170" s="74"/>
@@ -8151,11 +8152,11 @@
       <c r="D170" s="85"/>
       <c r="E170" s="86"/>
       <c r="F170" s="72"/>
-      <c r="G170" s="108"/>
+      <c r="G170" s="107"/>
       <c r="J170"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A171" s="107" t="s">
+      <c r="A171" s="106" t="s">
         <v>428</v>
       </c>
       <c r="B171" s="93"/>
@@ -8163,11 +8164,11 @@
       <c r="D171" s="97"/>
       <c r="E171" s="94"/>
       <c r="F171" s="72"/>
-      <c r="G171" s="111"/>
+      <c r="G171" s="110"/>
       <c r="J171"/>
     </row>
     <row r="172" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A172" s="107" t="s">
+      <c r="A172" s="106" t="s">
         <v>429</v>
       </c>
       <c r="B172" s="74"/>
@@ -8175,11 +8176,11 @@
       <c r="D172" s="85"/>
       <c r="E172" s="86"/>
       <c r="F172" s="72"/>
-      <c r="G172" s="108"/>
+      <c r="G172" s="107"/>
       <c r="J172"/>
     </row>
     <row r="173" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A173" s="107" t="s">
+      <c r="A173" s="106" t="s">
         <v>430</v>
       </c>
       <c r="B173" s="93"/>
@@ -8187,11 +8188,11 @@
       <c r="D173" s="97"/>
       <c r="E173" s="94"/>
       <c r="F173" s="72"/>
-      <c r="G173" s="111"/>
+      <c r="G173" s="110"/>
       <c r="J173"/>
     </row>
     <row r="174" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A174" s="107" t="s">
+      <c r="A174" s="106" t="s">
         <v>431</v>
       </c>
       <c r="B174" s="74"/>
@@ -8199,11 +8200,11 @@
       <c r="D174" s="85"/>
       <c r="E174" s="86"/>
       <c r="F174" s="72"/>
-      <c r="G174" s="108"/>
+      <c r="G174" s="107"/>
       <c r="J174"/>
     </row>
     <row r="175" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A175" s="107" t="s">
+      <c r="A175" s="106" t="s">
         <v>432</v>
       </c>
       <c r="B175" s="93"/>
@@ -8211,11 +8212,11 @@
       <c r="D175" s="97"/>
       <c r="E175" s="94"/>
       <c r="F175" s="72"/>
-      <c r="G175" s="111"/>
+      <c r="G175" s="110"/>
       <c r="J175"/>
     </row>
     <row r="176" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A176" s="107" t="s">
+      <c r="A176" s="106" t="s">
         <v>433</v>
       </c>
       <c r="B176" s="74"/>
@@ -8223,11 +8224,11 @@
       <c r="D176" s="85"/>
       <c r="E176" s="86"/>
       <c r="F176" s="72"/>
-      <c r="G176" s="108"/>
+      <c r="G176" s="107"/>
       <c r="J176"/>
     </row>
     <row r="177" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A177" s="107" t="s">
+      <c r="A177" s="106" t="s">
         <v>434</v>
       </c>
       <c r="B177" s="93"/>
@@ -8235,11 +8236,11 @@
       <c r="D177" s="97"/>
       <c r="E177" s="94"/>
       <c r="F177" s="72"/>
-      <c r="G177" s="111"/>
+      <c r="G177" s="110"/>
       <c r="J177"/>
     </row>
     <row r="178" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A178" s="107" t="s">
+      <c r="A178" s="106" t="s">
         <v>435</v>
       </c>
       <c r="B178" s="74"/>
@@ -8247,11 +8248,11 @@
       <c r="D178" s="85"/>
       <c r="E178" s="86"/>
       <c r="F178" s="72"/>
-      <c r="G178" s="108"/>
+      <c r="G178" s="107"/>
       <c r="J178"/>
     </row>
     <row r="179" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A179" s="107" t="s">
+      <c r="A179" s="106" t="s">
         <v>436</v>
       </c>
       <c r="B179" s="93"/>
@@ -8259,11 +8260,11 @@
       <c r="D179" s="97"/>
       <c r="E179" s="94"/>
       <c r="F179" s="72"/>
-      <c r="G179" s="111"/>
+      <c r="G179" s="110"/>
       <c r="J179"/>
     </row>
     <row r="180" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A180" s="107" t="s">
+      <c r="A180" s="106" t="s">
         <v>437</v>
       </c>
       <c r="B180" s="74"/>
@@ -8271,11 +8272,11 @@
       <c r="D180" s="85"/>
       <c r="E180" s="86"/>
       <c r="F180" s="72"/>
-      <c r="G180" s="108"/>
+      <c r="G180" s="107"/>
       <c r="J180"/>
     </row>
     <row r="181" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A181" s="107" t="s">
+      <c r="A181" s="106" t="s">
         <v>438</v>
       </c>
       <c r="B181" s="93"/>
@@ -8283,11 +8284,11 @@
       <c r="D181" s="97"/>
       <c r="E181" s="94"/>
       <c r="F181" s="72"/>
-      <c r="G181" s="111"/>
+      <c r="G181" s="110"/>
       <c r="J181"/>
     </row>
     <row r="182" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A182" s="107" t="s">
+      <c r="A182" s="106" t="s">
         <v>439</v>
       </c>
       <c r="B182" s="74"/>
@@ -8295,11 +8296,11 @@
       <c r="D182" s="85"/>
       <c r="E182" s="86"/>
       <c r="F182" s="72"/>
-      <c r="G182" s="108"/>
+      <c r="G182" s="107"/>
       <c r="J182"/>
     </row>
     <row r="183" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A183" s="107" t="s">
+      <c r="A183" s="106" t="s">
         <v>440</v>
       </c>
       <c r="B183" s="93"/>
@@ -8307,11 +8308,11 @@
       <c r="D183" s="97"/>
       <c r="E183" s="94"/>
       <c r="F183" s="72"/>
-      <c r="G183" s="111"/>
+      <c r="G183" s="110"/>
       <c r="J183"/>
     </row>
     <row r="184" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A184" s="107" t="s">
+      <c r="A184" s="106" t="s">
         <v>441</v>
       </c>
       <c r="B184" s="74"/>
@@ -8319,11 +8320,11 @@
       <c r="D184" s="85"/>
       <c r="E184" s="86"/>
       <c r="F184" s="72"/>
-      <c r="G184" s="108"/>
+      <c r="G184" s="107"/>
       <c r="J184"/>
     </row>
     <row r="185" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A185" s="107" t="s">
+      <c r="A185" s="106" t="s">
         <v>442</v>
       </c>
       <c r="B185" s="93"/>
@@ -8331,11 +8332,11 @@
       <c r="D185" s="97"/>
       <c r="E185" s="94"/>
       <c r="F185" s="72"/>
-      <c r="G185" s="111"/>
+      <c r="G185" s="110"/>
       <c r="J185"/>
     </row>
     <row r="186" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A186" s="107" t="s">
+      <c r="A186" s="106" t="s">
         <v>443</v>
       </c>
       <c r="B186" s="74"/>
@@ -8343,11 +8344,11 @@
       <c r="D186" s="85"/>
       <c r="E186" s="86"/>
       <c r="F186" s="72"/>
-      <c r="G186" s="108"/>
+      <c r="G186" s="107"/>
       <c r="J186"/>
     </row>
     <row r="187" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A187" s="107" t="s">
+      <c r="A187" s="106" t="s">
         <v>444</v>
       </c>
       <c r="B187" s="93"/>
@@ -8355,11 +8356,11 @@
       <c r="D187" s="97"/>
       <c r="E187" s="94"/>
       <c r="F187" s="72"/>
-      <c r="G187" s="111"/>
+      <c r="G187" s="110"/>
       <c r="J187"/>
     </row>
     <row r="188" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A188" s="107" t="s">
+      <c r="A188" s="106" t="s">
         <v>445</v>
       </c>
       <c r="B188" s="74"/>
@@ -8367,11 +8368,11 @@
       <c r="D188" s="85"/>
       <c r="E188" s="86"/>
       <c r="F188" s="72"/>
-      <c r="G188" s="108"/>
+      <c r="G188" s="107"/>
       <c r="J188"/>
     </row>
     <row r="189" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A189" s="107" t="s">
+      <c r="A189" s="106" t="s">
         <v>446</v>
       </c>
       <c r="B189" s="93"/>
@@ -8379,11 +8380,11 @@
       <c r="D189" s="97"/>
       <c r="E189" s="94"/>
       <c r="F189" s="72"/>
-      <c r="G189" s="111"/>
+      <c r="G189" s="110"/>
       <c r="J189"/>
     </row>
     <row r="190" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A190" s="107" t="s">
+      <c r="A190" s="106" t="s">
         <v>447</v>
       </c>
       <c r="B190" s="74"/>
@@ -8391,11 +8392,11 @@
       <c r="D190" s="85"/>
       <c r="E190" s="86"/>
       <c r="F190" s="72"/>
-      <c r="G190" s="108"/>
+      <c r="G190" s="107"/>
       <c r="J190"/>
     </row>
     <row r="191" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A191" s="107" t="s">
+      <c r="A191" s="106" t="s">
         <v>448</v>
       </c>
       <c r="B191" s="93"/>
@@ -8403,11 +8404,11 @@
       <c r="D191" s="97"/>
       <c r="E191" s="94"/>
       <c r="F191" s="72"/>
-      <c r="G191" s="111"/>
+      <c r="G191" s="110"/>
       <c r="J191"/>
     </row>
     <row r="192" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A192" s="107" t="s">
+      <c r="A192" s="106" t="s">
         <v>449</v>
       </c>
       <c r="B192" s="74"/>
@@ -8415,11 +8416,11 @@
       <c r="D192" s="85"/>
       <c r="E192" s="86"/>
       <c r="F192" s="72"/>
-      <c r="G192" s="108"/>
+      <c r="G192" s="107"/>
       <c r="J192"/>
     </row>
     <row r="193" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A193" s="107" t="s">
+      <c r="A193" s="106" t="s">
         <v>450</v>
       </c>
       <c r="B193" s="93"/>
@@ -8427,11 +8428,11 @@
       <c r="D193" s="97"/>
       <c r="E193" s="94"/>
       <c r="F193" s="72"/>
-      <c r="G193" s="111"/>
+      <c r="G193" s="110"/>
       <c r="J193"/>
     </row>
     <row r="194" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A194" s="107" t="s">
+      <c r="A194" s="106" t="s">
         <v>451</v>
       </c>
       <c r="B194" s="74"/>
@@ -8439,11 +8440,11 @@
       <c r="D194" s="85"/>
       <c r="E194" s="86"/>
       <c r="F194" s="72"/>
-      <c r="G194" s="108"/>
+      <c r="G194" s="107"/>
       <c r="J194"/>
     </row>
     <row r="195" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A195" s="107" t="s">
+      <c r="A195" s="106" t="s">
         <v>452</v>
       </c>
       <c r="B195" s="93"/>
@@ -8451,11 +8452,11 @@
       <c r="D195" s="97"/>
       <c r="E195" s="94"/>
       <c r="F195" s="72"/>
-      <c r="G195" s="111"/>
+      <c r="G195" s="110"/>
       <c r="J195"/>
     </row>
     <row r="196" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A196" s="107" t="s">
+      <c r="A196" s="106" t="s">
         <v>453</v>
       </c>
       <c r="B196" s="74"/>
@@ -8463,11 +8464,11 @@
       <c r="D196" s="85"/>
       <c r="E196" s="86"/>
       <c r="F196" s="72"/>
-      <c r="G196" s="108"/>
+      <c r="G196" s="107"/>
       <c r="J196"/>
     </row>
     <row r="197" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A197" s="107" t="s">
+      <c r="A197" s="106" t="s">
         <v>454</v>
       </c>
       <c r="B197" s="93"/>
@@ -8475,11 +8476,11 @@
       <c r="D197" s="97"/>
       <c r="E197" s="94"/>
       <c r="F197" s="72"/>
-      <c r="G197" s="111"/>
+      <c r="G197" s="110"/>
       <c r="J197"/>
     </row>
     <row r="198" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A198" s="107" t="s">
+      <c r="A198" s="106" t="s">
         <v>455</v>
       </c>
       <c r="B198" s="74"/>
@@ -8487,11 +8488,11 @@
       <c r="D198" s="85"/>
       <c r="E198" s="86"/>
       <c r="F198" s="72"/>
-      <c r="G198" s="108"/>
+      <c r="G198" s="107"/>
       <c r="J198"/>
     </row>
     <row r="199" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A199" s="107" t="s">
+      <c r="A199" s="106" t="s">
         <v>456</v>
       </c>
       <c r="B199" s="93"/>
@@ -8499,11 +8500,11 @@
       <c r="D199" s="97"/>
       <c r="E199" s="94"/>
       <c r="F199" s="72"/>
-      <c r="G199" s="111"/>
+      <c r="G199" s="110"/>
       <c r="J199"/>
     </row>
     <row r="200" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A200" s="107" t="s">
+      <c r="A200" s="106" t="s">
         <v>457</v>
       </c>
       <c r="B200" s="74"/>
@@ -8511,11 +8512,11 @@
       <c r="D200" s="85"/>
       <c r="E200" s="86"/>
       <c r="F200" s="72"/>
-      <c r="G200" s="108"/>
+      <c r="G200" s="107"/>
       <c r="J200"/>
     </row>
     <row r="201" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A201" s="107" t="s">
+      <c r="A201" s="106" t="s">
         <v>458</v>
       </c>
       <c r="B201" s="93"/>
@@ -8523,11 +8524,11 @@
       <c r="D201" s="97"/>
       <c r="E201" s="94"/>
       <c r="F201" s="72"/>
-      <c r="G201" s="111"/>
+      <c r="G201" s="110"/>
       <c r="J201"/>
     </row>
     <row r="202" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A202" s="107" t="s">
+      <c r="A202" s="106" t="s">
         <v>459</v>
       </c>
       <c r="B202" s="74"/>
@@ -8535,11 +8536,11 @@
       <c r="D202" s="85"/>
       <c r="E202" s="86"/>
       <c r="F202" s="72"/>
-      <c r="G202" s="108"/>
+      <c r="G202" s="107"/>
       <c r="J202"/>
     </row>
     <row r="203" spans="1:10" ht="15.75" hidden="1" customHeight="1">
-      <c r="A203" s="107" t="s">
+      <c r="A203" s="106" t="s">
         <v>460</v>
       </c>
       <c r="B203" s="93"/>
@@ -8547,11 +8548,11 @@
       <c r="D203" s="97"/>
       <c r="E203" s="94"/>
       <c r="F203" s="72"/>
-      <c r="G203" s="111"/>
+      <c r="G203" s="110"/>
       <c r="J203"/>
     </row>
     <row r="204" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A204" s="105" t="s">
+      <c r="A204" s="104" t="s">
         <v>362</v>
       </c>
       <c r="B204" s="75" t="s">
@@ -8567,13 +8568,13 @@
       <c r="F204" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G204" s="112" t="s">
+      <c r="G204" s="111" t="s">
         <v>464</v>
       </c>
       <c r="J204"/>
     </row>
     <row r="205" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A205" s="107" t="s">
+      <c r="A205" s="106" t="s">
         <v>363</v>
       </c>
       <c r="B205" s="74" t="s">
@@ -8589,13 +8590,13 @@
       <c r="F205" s="74" t="s">
         <v>467</v>
       </c>
-      <c r="G205" s="113" t="s">
+      <c r="G205" s="112" t="s">
         <v>334</v>
       </c>
       <c r="J205"/>
     </row>
     <row r="206" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A206" s="105" t="s">
+      <c r="A206" s="104" t="s">
         <v>364</v>
       </c>
       <c r="B206" s="75" t="s">
@@ -8611,13 +8612,13 @@
       <c r="F206" s="75" t="s">
         <v>470</v>
       </c>
-      <c r="G206" s="112" t="s">
+      <c r="G206" s="111" t="s">
         <v>471</v>
       </c>
       <c r="J206"/>
     </row>
     <row r="207" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A207" s="107" t="s">
+      <c r="A207" s="106" t="s">
         <v>365</v>
       </c>
       <c r="B207" s="72" t="s">
@@ -8633,13 +8634,13 @@
       <c r="F207" s="72" t="s">
         <v>474</v>
       </c>
-      <c r="G207" s="108" t="s">
+      <c r="G207" s="107" t="s">
         <v>475</v>
       </c>
       <c r="J207"/>
     </row>
     <row r="208" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A208" s="105" t="s">
+      <c r="A208" s="104" t="s">
         <v>366</v>
       </c>
       <c r="B208" s="71" t="s">
@@ -8655,13 +8656,13 @@
       <c r="F208" s="71" t="s">
         <v>478</v>
       </c>
-      <c r="G208" s="114" t="s">
+      <c r="G208" s="113" t="s">
         <v>479</v>
       </c>
       <c r="J208"/>
     </row>
     <row r="209" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A209" s="107" t="s">
+      <c r="A209" s="106" t="s">
         <v>367</v>
       </c>
       <c r="B209" s="72" t="s">
@@ -8677,13 +8678,13 @@
       <c r="F209" s="72" t="s">
         <v>482</v>
       </c>
-      <c r="G209" s="115" t="s">
+      <c r="G209" s="114" t="s">
         <v>479</v>
       </c>
       <c r="J209"/>
     </row>
     <row r="210" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A210" s="105" t="s">
+      <c r="A210" s="104" t="s">
         <v>368</v>
       </c>
       <c r="B210" s="71" t="s">
@@ -8699,13 +8700,13 @@
       <c r="F210" s="71" t="s">
         <v>485</v>
       </c>
-      <c r="G210" s="114" t="s">
+      <c r="G210" s="113" t="s">
         <v>486</v>
       </c>
       <c r="J210"/>
     </row>
     <row r="211" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A211" s="107" t="s">
+      <c r="A211" s="106" t="s">
         <v>369</v>
       </c>
       <c r="B211" s="72" t="s">
@@ -8721,13 +8722,13 @@
       <c r="F211" s="72" t="s">
         <v>661</v>
       </c>
-      <c r="G211" s="115" t="s">
+      <c r="G211" s="114" t="s">
         <v>660</v>
       </c>
       <c r="J211"/>
     </row>
     <row r="212" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A212" s="105" t="s">
+      <c r="A212" s="104" t="s">
         <v>370</v>
       </c>
       <c r="B212" s="71" t="s">
@@ -8743,13 +8744,13 @@
       <c r="F212" s="71" t="s">
         <v>714</v>
       </c>
-      <c r="G212" s="114" t="s">
+      <c r="G212" s="113" t="s">
         <v>713</v>
       </c>
       <c r="J212"/>
     </row>
     <row r="213" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A213" s="107" t="s">
+      <c r="A213" s="106" t="s">
         <v>371</v>
       </c>
       <c r="B213" s="72" t="s">
@@ -8765,13 +8766,13 @@
       <c r="F213" s="72" t="s">
         <v>715</v>
       </c>
-      <c r="G213" s="115" t="s">
+      <c r="G213" s="114" t="s">
         <v>712</v>
       </c>
       <c r="J213"/>
     </row>
     <row r="214" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A214" s="168" t="s">
+      <c r="A214" s="133" t="s">
         <v>372</v>
       </c>
       <c r="B214" s="71" t="s">
@@ -8787,13 +8788,13 @@
       <c r="F214" s="71" t="s">
         <v>716</v>
       </c>
-      <c r="G214" s="114" t="s">
+      <c r="G214" s="113" t="s">
         <v>711</v>
       </c>
       <c r="J214"/>
     </row>
     <row r="215" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A215" s="107" t="s">
+      <c r="A215" s="106" t="s">
         <v>373</v>
       </c>
       <c r="B215" s="72" t="s">
@@ -8809,37 +8810,37 @@
       <c r="F215" s="72" t="s">
         <v>719</v>
       </c>
-      <c r="G215" s="115" t="s">
+      <c r="G215" s="114" t="s">
         <v>720</v>
       </c>
       <c r="J215"/>
     </row>
     <row r="216" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A216" s="120" t="s">
+      <c r="A216" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B216" s="121" t="s">
+      <c r="B216" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="C216" s="122" t="s">
+      <c r="C216" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D216" s="123" t="s">
+      <c r="D216" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="E216" s="124" t="s">
+      <c r="E216" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="F216" s="125" t="s">
+      <c r="F216" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="G216" s="126" t="s">
+      <c r="G216" s="125" t="s">
         <v>7</v>
       </c>
       <c r="J216"/>
     </row>
     <row r="217" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A217" s="105" t="s">
+      <c r="A217" s="104" t="s">
         <v>374</v>
       </c>
       <c r="B217" s="71" t="s">
@@ -8855,13 +8856,13 @@
       <c r="F217" s="71" t="s">
         <v>730</v>
       </c>
-      <c r="G217" s="114" t="s">
+      <c r="G217" s="113" t="s">
         <v>728</v>
       </c>
       <c r="J217"/>
     </row>
     <row r="218" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A218" s="107" t="s">
+      <c r="A218" s="106" t="s">
         <v>375</v>
       </c>
       <c r="B218" s="72" t="s">
@@ -8877,13 +8878,13 @@
       <c r="F218" s="72" t="s">
         <v>731</v>
       </c>
-      <c r="G218" s="115" t="s">
+      <c r="G218" s="114" t="s">
         <v>729</v>
       </c>
       <c r="J218"/>
     </row>
     <row r="219" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A219" s="105" t="s">
+      <c r="A219" s="104" t="s">
         <v>376</v>
       </c>
       <c r="B219" s="71" t="s">
@@ -8899,29 +8900,29 @@
       <c r="F219" s="71" t="s">
         <v>732</v>
       </c>
-      <c r="G219" s="114" t="s">
+      <c r="G219" s="113" t="s">
         <v>727</v>
       </c>
       <c r="J219"/>
     </row>
     <row r="220" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A220" s="116" t="s">
+      <c r="A220" s="115" t="s">
         <v>377</v>
       </c>
-      <c r="B220" s="117" t="s">
+      <c r="B220" s="116" t="s">
         <v>726</v>
       </c>
-      <c r="C220" s="118">
+      <c r="C220" s="117">
         <v>2</v>
       </c>
-      <c r="D220" s="117"/>
-      <c r="E220" s="117" t="s">
+      <c r="D220" s="116"/>
+      <c r="E220" s="116" t="s">
         <v>738</v>
       </c>
-      <c r="F220" s="117" t="s">
+      <c r="F220" s="116" t="s">
         <v>733</v>
       </c>
-      <c r="G220" s="119" t="s">
+      <c r="G220" s="118" t="s">
         <v>734</v>
       </c>
       <c r="J220"/>
@@ -11820,10 +11821,14 @@
     <hyperlink ref="A214" r:id="rId1"/>
     <hyperlink ref="A85" r:id="rId2"/>
     <hyperlink ref="A79" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A14" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -11850,50 +11855,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="154" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="141"/>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="156"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="157" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="143"/>
+      <c r="B2" s="142"/>
       <c r="C2" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D2" s="144" t="s">
+      <c r="D2" s="158" t="s">
         <v>492</v>
       </c>
       <c r="E2" s="145"/>
       <c r="F2" s="145"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="146" t="s">
+      <c r="G2" s="142"/>
+      <c r="H2" s="159" t="s">
         <v>493</v>
       </c>
-      <c r="I2" s="147"/>
+      <c r="I2" s="146"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="160" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="140"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="140"/>
-      <c r="I4" s="141"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="156"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="8" t="s">
@@ -11955,15 +11960,15 @@
       <c r="I6" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="K6" s="149" t="s">
+      <c r="K6" s="148" t="s">
         <v>512</v>
       </c>
-      <c r="L6" s="150"/>
-      <c r="M6" s="150"/>
-      <c r="N6" s="150"/>
-      <c r="O6" s="150"/>
-      <c r="P6" s="150"/>
-      <c r="Q6" s="150"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="12">
@@ -11993,15 +11998,15 @@
       <c r="I7" s="14" t="s">
         <v>520</v>
       </c>
-      <c r="K7" s="149" t="s">
+      <c r="K7" s="148" t="s">
         <v>521</v>
       </c>
-      <c r="L7" s="150"/>
-      <c r="M7" s="150"/>
-      <c r="N7" s="150"/>
-      <c r="O7" s="150"/>
-      <c r="P7" s="150"/>
-      <c r="Q7" s="150"/>
+      <c r="L7" s="149"/>
+      <c r="M7" s="149"/>
+      <c r="N7" s="149"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="12">
@@ -12109,17 +12114,17 @@
       <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="150" t="s">
         <v>530</v>
       </c>
-      <c r="B15" s="152"/>
-      <c r="C15" s="152"/>
-      <c r="D15" s="152"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="152"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="153"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="152"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="8" t="s">
@@ -12134,15 +12139,15 @@
       <c r="D16" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="E16" s="154" t="s">
+      <c r="E16" s="153" t="s">
         <v>531</v>
       </c>
-      <c r="F16" s="155"/>
-      <c r="G16" s="154" t="s">
+      <c r="F16" s="140"/>
+      <c r="G16" s="153" t="s">
         <v>532</v>
       </c>
-      <c r="H16" s="156"/>
-      <c r="I16" s="157"/>
+      <c r="H16" s="143"/>
+      <c r="I16" s="144"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="19">
@@ -12157,15 +12162,15 @@
       <c r="D17" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="E17" s="158" t="s">
+      <c r="E17" s="147" t="s">
         <v>534</v>
       </c>
-      <c r="F17" s="155"/>
-      <c r="G17" s="158" t="s">
+      <c r="F17" s="140"/>
+      <c r="G17" s="147" t="s">
         <v>535</v>
       </c>
-      <c r="H17" s="156"/>
-      <c r="I17" s="157"/>
+      <c r="H17" s="143"/>
+      <c r="I17" s="144"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="19">
@@ -12180,15 +12185,15 @@
       <c r="D18" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="E18" s="158" t="s">
+      <c r="E18" s="147" t="s">
         <v>534</v>
       </c>
-      <c r="F18" s="155"/>
-      <c r="G18" s="158" t="s">
+      <c r="F18" s="140"/>
+      <c r="G18" s="147" t="s">
         <v>537</v>
       </c>
-      <c r="H18" s="156"/>
-      <c r="I18" s="157"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="144"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="19">
@@ -12203,15 +12208,15 @@
       <c r="D19" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="E19" s="158" t="s">
+      <c r="E19" s="147" t="s">
         <v>540</v>
       </c>
-      <c r="F19" s="155"/>
-      <c r="G19" s="158" t="s">
+      <c r="F19" s="140"/>
+      <c r="G19" s="147" t="s">
         <v>541</v>
       </c>
-      <c r="H19" s="156"/>
-      <c r="I19" s="157"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="144"/>
       <c r="K19" s="11" t="s">
         <v>542</v>
       </c>
@@ -12223,11 +12228,11 @@
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="155"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="157"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="143"/>
+      <c r="I20" s="144"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="19">
@@ -12236,11 +12241,11 @@
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="159"/>
-      <c r="F21" s="155"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="156"/>
-      <c r="I21" s="157"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="144"/>
       <c r="K21" s="11" t="s">
         <v>543</v>
       </c>
@@ -12252,11 +12257,11 @@
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="159"/>
-      <c r="F22" s="155"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="156"/>
-      <c r="I22" s="157"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="144"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="19">
@@ -12265,11 +12270,11 @@
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="155"/>
-      <c r="G23" s="159"/>
-      <c r="H23" s="156"/>
-      <c r="I23" s="157"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="140"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="144"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="19">
@@ -12278,11 +12283,11 @@
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="155"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="157"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="140"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="143"/>
+      <c r="I24" s="144"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="19">
@@ -12291,11 +12296,11 @@
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="159"/>
-      <c r="F25" s="155"/>
-      <c r="G25" s="159"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="157"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="143"/>
+      <c r="I25" s="144"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="21">
@@ -12304,11 +12309,11 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="160"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="160"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="141"/>
       <c r="H26" s="145"/>
-      <c r="I26" s="147"/>
+      <c r="I26" s="146"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -13286,14 +13291,16 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -13306,16 +13313,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16466,7 +16471,7 @@
       <c r="B2" s="164" t="s">
         <v>554</v>
       </c>
-      <c r="C2" s="155"/>
+      <c r="C2" s="140"/>
       <c r="O2" s="11" t="s">
         <v>555</v>
       </c>
@@ -17683,8 +17688,8 @@
       <c r="A3" s="164" t="s">
         <v>587</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="155"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="43" t="s">
@@ -17693,7 +17698,7 @@
       <c r="B4" s="166" t="s">
         <v>588</v>
       </c>
-      <c r="C4" s="155"/>
+      <c r="C4" s="140"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="44" t="s">
@@ -17702,7 +17707,7 @@
       <c r="B5" s="165" t="s">
         <v>590</v>
       </c>
-      <c r="C5" s="155"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="44" t="s">
@@ -17711,7 +17716,7 @@
       <c r="B6" s="165" t="s">
         <v>592</v>
       </c>
-      <c r="C6" s="155"/>
+      <c r="C6" s="140"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="44" t="s">
@@ -17720,7 +17725,7 @@
       <c r="B7" s="165" t="s">
         <v>594</v>
       </c>
-      <c r="C7" s="155"/>
+      <c r="C7" s="140"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="44" t="s">
@@ -17729,7 +17734,7 @@
       <c r="B8" s="165" t="s">
         <v>596</v>
       </c>
-      <c r="C8" s="155"/>
+      <c r="C8" s="140"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -18760,8 +18765,8 @@
       <c r="B2" s="167" t="s">
         <v>597</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="141"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="156"/>
       <c r="J2" s="11" t="s">
         <v>555</v>
       </c>
@@ -22913,8 +22918,8 @@
       <c r="A5" s="166" t="s">
         <v>630</v>
       </c>
-      <c r="B5" s="156"/>
-      <c r="C5" s="155"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="43" t="s">

</xml_diff>

<commit_message>
chg: Update TGT list with links to tgt folders
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/OPAC Joint Target List.xlsx
+++ b/INTELLIGENCE/OPAC Joint Target List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="771">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2356,12 +2356,15 @@
   <si>
     <t>882ft</t>
   </si>
+  <si>
+    <t>Poliarnie Ammunition Factory</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2551,6 +2554,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3568,9 +3578,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3595,9 +3602,6 @@
     <xf numFmtId="0" fontId="28" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3611,6 +3615,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="6" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3620,20 +3627,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3647,22 +3659,17 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3681,8 +3688,9 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
@@ -3717,7 +3725,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3751,7 +3759,7 @@
         <xdr:cNvPr id="3" name="image2.png" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3790,7 +3798,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3824,7 +3832,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3863,7 +3871,7 @@
         <xdr:cNvPr id="2" name="image10.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3897,7 +3905,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3936,7 +3944,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4093,7 +4101,7 @@
         <xdr:cNvPr id="4" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4127,7 +4135,7 @@
         <xdr:cNvPr id="5" name="image6.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4166,7 +4174,7 @@
         <xdr:cNvPr id="4" name="Shape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4323,7 +4331,7 @@
         <xdr:cNvPr id="3" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4357,7 +4365,7 @@
         <xdr:cNvPr id="5" name="image9.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4396,7 +4404,7 @@
         <xdr:cNvPr id="5" name="Shape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4577,7 +4585,7 @@
         <xdr:cNvPr id="3" name="image7.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4611,7 +4619,7 @@
         <xdr:cNvPr id="4" name="image14.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4650,7 +4658,7 @@
         <xdr:cNvPr id="6" name="Shape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4771,7 +4779,7 @@
         <xdr:cNvPr id="3" name="image13.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4805,7 +4813,7 @@
         <xdr:cNvPr id="4" name="image11.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4839,7 +4847,7 @@
         <xdr:cNvPr id="5" name="image12.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5061,13 +5069,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J998"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5086,22 +5094,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="49.5" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="136"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="137"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="138" t="s">
         <v>739</v>
       </c>
-      <c r="B2" s="138"/>
+      <c r="B2" s="139"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -5134,7 +5142,7 @@
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" ht="14.25">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="133" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="76" t="s">
@@ -5178,7 +5186,7 @@
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" ht="14.25">
-      <c r="A6" s="169" t="s">
+      <c r="A6" s="134" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="74" t="s">
@@ -5200,7 +5208,7 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="14.25">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="131" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="75" t="s">
@@ -5222,7 +5230,7 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" ht="14.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="134" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="74" t="s">
@@ -5362,7 +5370,7 @@
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" ht="14.25">
-      <c r="A14" s="169" t="s">
+      <c r="A14" s="134" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="74" t="s">
@@ -5384,7 +5392,7 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" ht="14.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="131" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="75" t="s">
@@ -5406,7 +5414,7 @@
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" ht="14.25">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="134" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="74" t="s">
@@ -5428,7 +5436,7 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" ht="14.25">
-      <c r="A17" s="104" t="s">
+      <c r="A17" s="131" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="75" t="s">
@@ -5450,7 +5458,7 @@
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" ht="14.25">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="134" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="74" t="s">
@@ -5472,7 +5480,7 @@
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" ht="14.25">
-      <c r="A19" s="104" t="s">
+      <c r="A19" s="131" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="75" t="s">
@@ -5494,7 +5502,7 @@
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" ht="14.25">
-      <c r="A20" s="106" t="s">
+      <c r="A20" s="134" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="74" t="s">
@@ -5538,7 +5546,7 @@
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A22" s="106" t="s">
+      <c r="A22" s="134" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="74" t="s">
@@ -5560,7 +5568,7 @@
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="131" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="75" t="s">
@@ -5582,7 +5590,7 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A24" s="106" t="s">
+      <c r="A24" s="134" t="s">
         <v>95</v>
       </c>
       <c r="B24" s="74" t="s">
@@ -5648,7 +5656,7 @@
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="104" t="s">
+      <c r="A27" s="131" t="s">
         <v>109</v>
       </c>
       <c r="B27" s="75" t="s">
@@ -5670,7 +5678,7 @@
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="134" t="s">
         <v>112</v>
       </c>
       <c r="B28" s="74" t="s">
@@ -5692,7 +5700,7 @@
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="131" t="s">
         <v>113</v>
       </c>
       <c r="B29" s="75" t="s">
@@ -5714,7 +5722,7 @@
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="106" t="s">
+      <c r="A30" s="134" t="s">
         <v>114</v>
       </c>
       <c r="B30" s="74" t="s">
@@ -5890,25 +5898,25 @@
       <c r="J37"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="128" t="s">
+      <c r="A38" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="129" t="s">
+      <c r="B38" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="126" t="s">
+      <c r="C38" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="127" t="s">
+      <c r="D38" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="130" t="s">
+      <c r="E38" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="131" t="s">
+      <c r="F38" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="132" t="s">
+      <c r="G38" s="130" t="s">
         <v>7</v>
       </c>
       <c r="J38"/>
@@ -6134,7 +6142,7 @@
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A49" s="106" t="s">
+      <c r="A49" s="134" t="s">
         <v>180</v>
       </c>
       <c r="B49" s="74" t="s">
@@ -6156,7 +6164,7 @@
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A50" s="104" t="s">
+      <c r="A50" s="131" t="s">
         <v>183</v>
       </c>
       <c r="B50" s="75" t="s">
@@ -6178,7 +6186,7 @@
       <c r="J50"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A51" s="106" t="s">
+      <c r="A51" s="134" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="74" t="s">
@@ -6244,7 +6252,7 @@
       <c r="J53"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A54" s="104" t="s">
+      <c r="A54" s="131" t="s">
         <v>195</v>
       </c>
       <c r="B54" s="75" t="s">
@@ -6266,7 +6274,7 @@
       <c r="J54"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A55" s="106" t="s">
+      <c r="A55" s="134" t="s">
         <v>198</v>
       </c>
       <c r="B55" s="74" t="s">
@@ -6288,7 +6296,7 @@
       <c r="J55"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A56" s="104" t="s">
+      <c r="A56" s="131" t="s">
         <v>200</v>
       </c>
       <c r="B56" s="75" t="s">
@@ -6332,7 +6340,7 @@
       <c r="J57"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A58" s="104" t="s">
+      <c r="A58" s="131" t="s">
         <v>208</v>
       </c>
       <c r="B58" s="75" t="s">
@@ -6376,7 +6384,7 @@
       <c r="J59"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A60" s="104" t="s">
+      <c r="A60" s="131" t="s">
         <v>215</v>
       </c>
       <c r="B60" s="75" t="s">
@@ -6420,7 +6428,7 @@
       <c r="J61"/>
     </row>
     <row r="62" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A62" s="104" t="s">
+      <c r="A62" s="131" t="s">
         <v>220</v>
       </c>
       <c r="B62" s="75" t="s">
@@ -6464,7 +6472,7 @@
       <c r="J63"/>
     </row>
     <row r="64" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A64" s="104" t="s">
+      <c r="A64" s="131" t="s">
         <v>226</v>
       </c>
       <c r="B64" s="75" t="s">
@@ -6684,7 +6692,7 @@
       <c r="J73"/>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A74" s="104" t="s">
+      <c r="A74" s="131" t="s">
         <v>254</v>
       </c>
       <c r="B74" s="75" t="s">
@@ -6706,7 +6714,7 @@
       <c r="J74"/>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A75" s="106" t="s">
+      <c r="A75" s="134" t="s">
         <v>256</v>
       </c>
       <c r="B75" s="74" t="s">
@@ -6726,31 +6734,31 @@
       <c r="J75"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A76" s="119" t="s">
+      <c r="A76" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="120" t="s">
+      <c r="B76" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="126" t="s">
+      <c r="C76" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="127" t="s">
+      <c r="D76" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="123" t="s">
+      <c r="E76" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="124" t="s">
+      <c r="F76" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="G76" s="125" t="s">
+      <c r="G76" s="124" t="s">
         <v>7</v>
       </c>
       <c r="J76"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A77" s="104" t="s">
+      <c r="A77" s="131" t="s">
         <v>260</v>
       </c>
       <c r="B77" s="75" t="s">
@@ -6770,7 +6778,7 @@
       <c r="J77"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A78" s="106" t="s">
+      <c r="A78" s="134" t="s">
         <v>264</v>
       </c>
       <c r="B78" s="74" t="s">
@@ -6792,7 +6800,7 @@
       <c r="J78"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A79" s="133" t="s">
+      <c r="A79" s="131" t="s">
         <v>269</v>
       </c>
       <c r="B79" s="75" t="s">
@@ -6924,7 +6932,7 @@
       <c r="J84"/>
     </row>
     <row r="85" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A85" s="133" t="s">
+      <c r="A85" s="131" t="s">
         <v>287</v>
       </c>
       <c r="B85" s="75" t="s">
@@ -7122,7 +7130,7 @@
       <c r="J93"/>
     </row>
     <row r="94" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A94" s="106" t="s">
+      <c r="A94" s="134" t="s">
         <v>315</v>
       </c>
       <c r="B94" s="74" t="s">
@@ -7166,7 +7174,7 @@
       <c r="J95"/>
     </row>
     <row r="96" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A96" s="106" t="s">
+      <c r="A96" s="134" t="s">
         <v>323</v>
       </c>
       <c r="B96" s="74" t="s">
@@ -7188,7 +7196,7 @@
       <c r="J96"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A97" s="104" t="s">
+      <c r="A97" s="131" t="s">
         <v>327</v>
       </c>
       <c r="B97" s="75" t="s">
@@ -7232,7 +7240,7 @@
       <c r="J98"/>
     </row>
     <row r="99" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A99" s="104" t="s">
+      <c r="A99" s="131" t="s">
         <v>335</v>
       </c>
       <c r="B99" s="75" t="s">
@@ -7254,7 +7262,7 @@
       <c r="J99"/>
     </row>
     <row r="100" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A100" s="106" t="s">
+      <c r="A100" s="134" t="s">
         <v>339</v>
       </c>
       <c r="B100" s="74" t="s">
@@ -7276,7 +7284,7 @@
       <c r="J100"/>
     </row>
     <row r="101" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A101" s="104" t="s">
+      <c r="A101" s="131" t="s">
         <v>344</v>
       </c>
       <c r="B101" s="75" t="s">
@@ -7298,7 +7306,7 @@
       <c r="J101"/>
     </row>
     <row r="102" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A102" s="106" t="s">
+      <c r="A102" s="134" t="s">
         <v>348</v>
       </c>
       <c r="B102" s="74" t="s">
@@ -8551,390 +8559,402 @@
       <c r="G203" s="110"/>
       <c r="J203"/>
     </row>
-    <row r="204" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A204" s="104" t="s">
+    <row r="204" spans="1:10" s="132" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A204" s="106"/>
+      <c r="B204" s="93"/>
+      <c r="C204" s="96"/>
+      <c r="D204" s="97"/>
+      <c r="E204" s="94"/>
+      <c r="F204" s="72"/>
+      <c r="G204" s="110"/>
+    </row>
+    <row r="205" spans="1:10" s="132" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A205" s="134" t="s">
+        <v>358</v>
+      </c>
+      <c r="B205" s="93" t="s">
+        <v>770</v>
+      </c>
+      <c r="C205" s="96"/>
+      <c r="D205" s="97"/>
+      <c r="E205" s="94"/>
+      <c r="F205" s="72"/>
+      <c r="G205" s="110"/>
+    </row>
+    <row r="206" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A206" s="131" t="s">
         <v>362</v>
       </c>
-      <c r="B204" s="75" t="s">
+      <c r="B206" s="75" t="s">
         <v>461</v>
       </c>
-      <c r="C204" s="80">
+      <c r="C206" s="80">
         <v>9</v>
       </c>
-      <c r="D204" s="71"/>
-      <c r="E204" s="82" t="s">
+      <c r="D206" s="71"/>
+      <c r="E206" s="82" t="s">
         <v>462</v>
       </c>
-      <c r="F204" s="71" t="s">
+      <c r="F206" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G204" s="111" t="s">
+      <c r="G206" s="111" t="s">
         <v>464</v>
       </c>
-      <c r="J204"/>
-    </row>
-    <row r="205" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A205" s="106" t="s">
+      <c r="J206"/>
+    </row>
+    <row r="207" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A207" s="134" t="s">
         <v>363</v>
       </c>
-      <c r="B205" s="74" t="s">
+      <c r="B207" s="74" t="s">
         <v>465</v>
       </c>
-      <c r="C205" s="84">
+      <c r="C207" s="84">
         <v>9</v>
       </c>
-      <c r="D205" s="74"/>
-      <c r="E205" s="74" t="s">
+      <c r="D207" s="74"/>
+      <c r="E207" s="74" t="s">
         <v>466</v>
       </c>
-      <c r="F205" s="74" t="s">
+      <c r="F207" s="74" t="s">
         <v>467</v>
       </c>
-      <c r="G205" s="112" t="s">
+      <c r="G207" s="112" t="s">
         <v>334</v>
       </c>
-      <c r="J205"/>
-    </row>
-    <row r="206" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A206" s="104" t="s">
+      <c r="J207"/>
+    </row>
+    <row r="208" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A208" s="131" t="s">
         <v>364</v>
       </c>
-      <c r="B206" s="75" t="s">
+      <c r="B208" s="75" t="s">
         <v>468</v>
       </c>
-      <c r="C206" s="98">
+      <c r="C208" s="98">
         <v>9</v>
       </c>
-      <c r="D206" s="75"/>
-      <c r="E206" s="75" t="s">
+      <c r="D208" s="75"/>
+      <c r="E208" s="75" t="s">
         <v>469</v>
       </c>
-      <c r="F206" s="75" t="s">
+      <c r="F208" s="75" t="s">
         <v>470</v>
       </c>
-      <c r="G206" s="111" t="s">
+      <c r="G208" s="111" t="s">
         <v>471</v>
       </c>
-      <c r="J206"/>
-    </row>
-    <row r="207" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A207" s="106" t="s">
+      <c r="J208"/>
+    </row>
+    <row r="209" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A209" s="134" t="s">
         <v>365</v>
       </c>
-      <c r="B207" s="72" t="s">
+      <c r="B209" s="72" t="s">
         <v>472</v>
       </c>
-      <c r="C207" s="99">
+      <c r="C209" s="99">
         <v>9</v>
-      </c>
-      <c r="D207" s="72"/>
-      <c r="E207" s="72" t="s">
-        <v>473</v>
-      </c>
-      <c r="F207" s="72" t="s">
-        <v>474</v>
-      </c>
-      <c r="G207" s="107" t="s">
-        <v>475</v>
-      </c>
-      <c r="J207"/>
-    </row>
-    <row r="208" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A208" s="104" t="s">
-        <v>366</v>
-      </c>
-      <c r="B208" s="71" t="s">
-        <v>476</v>
-      </c>
-      <c r="C208" s="100">
-        <v>11</v>
-      </c>
-      <c r="D208" s="71"/>
-      <c r="E208" s="71" t="s">
-        <v>477</v>
-      </c>
-      <c r="F208" s="71" t="s">
-        <v>478</v>
-      </c>
-      <c r="G208" s="113" t="s">
-        <v>479</v>
-      </c>
-      <c r="J208"/>
-    </row>
-    <row r="209" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A209" s="106" t="s">
-        <v>367</v>
-      </c>
-      <c r="B209" s="72" t="s">
-        <v>480</v>
-      </c>
-      <c r="C209" s="99">
-        <v>11</v>
       </c>
       <c r="D209" s="72"/>
       <c r="E209" s="72" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="F209" s="72" t="s">
-        <v>482</v>
-      </c>
-      <c r="G209" s="114" t="s">
-        <v>479</v>
+        <v>474</v>
+      </c>
+      <c r="G209" s="107" t="s">
+        <v>475</v>
       </c>
       <c r="J209"/>
     </row>
     <row r="210" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A210" s="104" t="s">
-        <v>368</v>
+      <c r="A210" s="131" t="s">
+        <v>366</v>
       </c>
       <c r="B210" s="71" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="C210" s="100">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D210" s="71"/>
       <c r="E210" s="71" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="F210" s="71" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="G210" s="113" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="J210"/>
     </row>
     <row r="211" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A211" s="106" t="s">
-        <v>369</v>
+      <c r="A211" s="134" t="s">
+        <v>367</v>
       </c>
       <c r="B211" s="72" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="C211" s="99">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D211" s="72"/>
       <c r="E211" s="72" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="F211" s="72" t="s">
-        <v>661</v>
+        <v>482</v>
       </c>
       <c r="G211" s="114" t="s">
-        <v>660</v>
+        <v>479</v>
       </c>
       <c r="J211"/>
     </row>
     <row r="212" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A212" s="104" t="s">
-        <v>370</v>
+      <c r="A212" s="131" t="s">
+        <v>368</v>
       </c>
       <c r="B212" s="71" t="s">
-        <v>706</v>
+        <v>483</v>
       </c>
       <c r="C212" s="100">
         <v>2</v>
       </c>
       <c r="D212" s="71"/>
       <c r="E212" s="71" t="s">
-        <v>707</v>
+        <v>484</v>
       </c>
       <c r="F212" s="71" t="s">
-        <v>714</v>
+        <v>485</v>
       </c>
       <c r="G212" s="113" t="s">
-        <v>713</v>
+        <v>486</v>
       </c>
       <c r="J212"/>
     </row>
     <row r="213" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A213" s="106" t="s">
-        <v>371</v>
+      <c r="A213" s="134" t="s">
+        <v>369</v>
       </c>
       <c r="B213" s="72" t="s">
-        <v>708</v>
+        <v>487</v>
       </c>
       <c r="C213" s="99">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D213" s="72"/>
       <c r="E213" s="72" t="s">
-        <v>710</v>
+        <v>488</v>
       </c>
       <c r="F213" s="72" t="s">
-        <v>715</v>
+        <v>661</v>
       </c>
       <c r="G213" s="114" t="s">
-        <v>712</v>
+        <v>660</v>
       </c>
       <c r="J213"/>
     </row>
     <row r="214" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A214" s="133" t="s">
-        <v>372</v>
+      <c r="A214" s="131" t="s">
+        <v>370</v>
       </c>
       <c r="B214" s="71" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C214" s="100">
         <v>2</v>
       </c>
       <c r="D214" s="71"/>
       <c r="E214" s="71" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F214" s="71" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G214" s="113" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="J214"/>
     </row>
-    <row r="215" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A215" s="106" t="s">
-        <v>373</v>
+    <row r="215" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A215" s="134" t="s">
+        <v>371</v>
       </c>
       <c r="B215" s="72" t="s">
-        <v>717</v>
-      </c>
-      <c r="C215" s="101">
+        <v>708</v>
+      </c>
+      <c r="C215" s="99">
         <v>2</v>
       </c>
       <c r="D215" s="72"/>
       <c r="E215" s="72" t="s">
+        <v>710</v>
+      </c>
+      <c r="F215" s="72" t="s">
+        <v>715</v>
+      </c>
+      <c r="G215" s="114" t="s">
+        <v>712</v>
+      </c>
+      <c r="J215"/>
+    </row>
+    <row r="216" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A216" s="131" t="s">
+        <v>372</v>
+      </c>
+      <c r="B216" s="71" t="s">
+        <v>709</v>
+      </c>
+      <c r="C216" s="100">
+        <v>2</v>
+      </c>
+      <c r="D216" s="71"/>
+      <c r="E216" s="71" t="s">
+        <v>710</v>
+      </c>
+      <c r="F216" s="71" t="s">
+        <v>716</v>
+      </c>
+      <c r="G216" s="113" t="s">
+        <v>711</v>
+      </c>
+      <c r="J216"/>
+    </row>
+    <row r="217" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A217" s="106" t="s">
+        <v>373</v>
+      </c>
+      <c r="B217" s="72" t="s">
+        <v>717</v>
+      </c>
+      <c r="C217" s="101">
+        <v>2</v>
+      </c>
+      <c r="D217" s="72"/>
+      <c r="E217" s="72" t="s">
         <v>718</v>
       </c>
-      <c r="F215" s="72" t="s">
+      <c r="F217" s="72" t="s">
         <v>719</v>
       </c>
-      <c r="G215" s="114" t="s">
+      <c r="G217" s="114" t="s">
         <v>720</v>
       </c>
-      <c r="J215"/>
-    </row>
-    <row r="216" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A216" s="119" t="s">
+      <c r="J217"/>
+    </row>
+    <row r="218" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A218" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="B216" s="120" t="s">
+      <c r="B218" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C216" s="121" t="s">
+      <c r="C218" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="D216" s="122" t="s">
+      <c r="D218" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="E216" s="123" t="s">
+      <c r="E218" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="F216" s="124" t="s">
+      <c r="F218" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="G216" s="125" t="s">
+      <c r="G218" s="124" t="s">
         <v>7</v>
-      </c>
-      <c r="J216"/>
-    </row>
-    <row r="217" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A217" s="104" t="s">
-        <v>374</v>
-      </c>
-      <c r="B217" s="71" t="s">
-        <v>723</v>
-      </c>
-      <c r="C217" s="100">
-        <v>2</v>
-      </c>
-      <c r="D217" s="71"/>
-      <c r="E217" s="71" t="s">
-        <v>735</v>
-      </c>
-      <c r="F217" s="71" t="s">
-        <v>730</v>
-      </c>
-      <c r="G217" s="113" t="s">
-        <v>728</v>
-      </c>
-      <c r="J217"/>
-    </row>
-    <row r="218" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A218" s="106" t="s">
-        <v>375</v>
-      </c>
-      <c r="B218" s="72" t="s">
-        <v>724</v>
-      </c>
-      <c r="C218" s="99">
-        <v>2</v>
-      </c>
-      <c r="D218" s="72"/>
-      <c r="E218" s="72" t="s">
-        <v>736</v>
-      </c>
-      <c r="F218" s="72" t="s">
-        <v>731</v>
-      </c>
-      <c r="G218" s="114" t="s">
-        <v>729</v>
       </c>
       <c r="J218"/>
     </row>
     <row r="219" spans="1:10" ht="15.75" customHeight="1">
       <c r="A219" s="104" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B219" s="71" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C219" s="100">
         <v>2</v>
       </c>
       <c r="D219" s="71"/>
       <c r="E219" s="71" t="s">
+        <v>735</v>
+      </c>
+      <c r="F219" s="71" t="s">
+        <v>730</v>
+      </c>
+      <c r="G219" s="113" t="s">
+        <v>728</v>
+      </c>
+      <c r="J219"/>
+    </row>
+    <row r="220" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A220" s="106" t="s">
+        <v>375</v>
+      </c>
+      <c r="B220" s="72" t="s">
+        <v>724</v>
+      </c>
+      <c r="C220" s="99">
+        <v>2</v>
+      </c>
+      <c r="D220" s="72"/>
+      <c r="E220" s="72" t="s">
+        <v>736</v>
+      </c>
+      <c r="F220" s="72" t="s">
+        <v>731</v>
+      </c>
+      <c r="G220" s="114" t="s">
+        <v>729</v>
+      </c>
+      <c r="J220"/>
+    </row>
+    <row r="221" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A221" s="104" t="s">
+        <v>376</v>
+      </c>
+      <c r="B221" s="71" t="s">
+        <v>725</v>
+      </c>
+      <c r="C221" s="100">
+        <v>2</v>
+      </c>
+      <c r="D221" s="71"/>
+      <c r="E221" s="71" t="s">
         <v>737</v>
       </c>
-      <c r="F219" s="71" t="s">
+      <c r="F221" s="71" t="s">
         <v>732</v>
       </c>
-      <c r="G219" s="113" t="s">
+      <c r="G221" s="113" t="s">
         <v>727</v>
       </c>
-      <c r="J219"/>
-    </row>
-    <row r="220" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A220" s="115" t="s">
+      <c r="J221"/>
+    </row>
+    <row r="222" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A222" s="115" t="s">
         <v>377</v>
       </c>
-      <c r="B220" s="116" t="s">
+      <c r="B222" s="116" t="s">
         <v>726</v>
       </c>
-      <c r="C220" s="117">
+      <c r="C222" s="117">
         <v>2</v>
       </c>
-      <c r="D220" s="116"/>
-      <c r="E220" s="116" t="s">
+      <c r="D222" s="116"/>
+      <c r="E222" s="116" t="s">
         <v>738</v>
       </c>
-      <c r="F220" s="116" t="s">
+      <c r="F222" s="116" t="s">
         <v>733</v>
       </c>
-      <c r="G220" s="118" t="s">
+      <c r="G222" s="118" t="s">
         <v>734</v>
       </c>
-      <c r="J220"/>
-    </row>
-    <row r="221" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A221" s="6"/>
-      <c r="B221" s="63"/>
-      <c r="J221"/>
-    </row>
-    <row r="222" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A222" s="6"/>
-      <c r="B222" s="63"/>
       <c r="J222"/>
     </row>
     <row r="223" spans="1:10" ht="15.75" customHeight="1">
@@ -10067,67 +10087,69 @@
       <c r="B448" s="63"/>
       <c r="J448"/>
     </row>
-    <row r="449" spans="2:10" ht="15.75" customHeight="1">
+    <row r="449" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A449" s="6"/>
       <c r="B449" s="63"/>
       <c r="J449"/>
     </row>
-    <row r="450" spans="2:10" ht="15.75" customHeight="1">
+    <row r="450" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A450" s="6"/>
       <c r="B450" s="63"/>
       <c r="J450"/>
     </row>
-    <row r="451" spans="2:10" ht="15.75" customHeight="1">
+    <row r="451" spans="1:10" ht="15.75" customHeight="1">
       <c r="B451" s="63"/>
       <c r="J451"/>
     </row>
-    <row r="452" spans="2:10" ht="15.75" customHeight="1">
+    <row r="452" spans="1:10" ht="15.75" customHeight="1">
       <c r="B452" s="63"/>
       <c r="J452"/>
     </row>
-    <row r="453" spans="2:10" ht="15.75" customHeight="1">
+    <row r="453" spans="1:10" ht="15.75" customHeight="1">
       <c r="B453" s="63"/>
       <c r="J453"/>
     </row>
-    <row r="454" spans="2:10" ht="15.75" customHeight="1">
+    <row r="454" spans="1:10" ht="15.75" customHeight="1">
       <c r="B454" s="63"/>
       <c r="J454"/>
     </row>
-    <row r="455" spans="2:10" ht="15.75" customHeight="1">
+    <row r="455" spans="1:10" ht="15.75" customHeight="1">
       <c r="B455" s="63"/>
       <c r="J455"/>
     </row>
-    <row r="456" spans="2:10" ht="15.75" customHeight="1">
+    <row r="456" spans="1:10" ht="15.75" customHeight="1">
       <c r="B456" s="63"/>
       <c r="J456"/>
     </row>
-    <row r="457" spans="2:10" ht="15.75" customHeight="1">
+    <row r="457" spans="1:10" ht="15.75" customHeight="1">
       <c r="B457" s="63"/>
       <c r="J457"/>
     </row>
-    <row r="458" spans="2:10" ht="15.75" customHeight="1">
+    <row r="458" spans="1:10" ht="15.75" customHeight="1">
       <c r="B458" s="63"/>
       <c r="J458"/>
     </row>
-    <row r="459" spans="2:10" ht="15.75" customHeight="1">
+    <row r="459" spans="1:10" ht="15.75" customHeight="1">
       <c r="B459" s="63"/>
       <c r="J459"/>
     </row>
-    <row r="460" spans="2:10" ht="15.75" customHeight="1">
+    <row r="460" spans="1:10" ht="15.75" customHeight="1">
       <c r="B460" s="63"/>
       <c r="J460"/>
     </row>
-    <row r="461" spans="2:10" ht="15.75" customHeight="1">
+    <row r="461" spans="1:10" ht="15.75" customHeight="1">
       <c r="B461" s="63"/>
       <c r="J461"/>
     </row>
-    <row r="462" spans="2:10" ht="15.75" customHeight="1">
+    <row r="462" spans="1:10" ht="15.75" customHeight="1">
       <c r="B462" s="63"/>
       <c r="J462"/>
     </row>
-    <row r="463" spans="2:10" ht="15.75" customHeight="1">
+    <row r="463" spans="1:10" ht="15.75" customHeight="1">
       <c r="B463" s="63"/>
       <c r="J463"/>
     </row>
-    <row r="464" spans="2:10" ht="15.75" customHeight="1">
+    <row r="464" spans="1:10" ht="15.75" customHeight="1">
       <c r="B464" s="63"/>
       <c r="J464"/>
     </row>
@@ -10592,9 +10614,11 @@
       <c r="J579"/>
     </row>
     <row r="580" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B580" s="63"/>
       <c r="J580"/>
     </row>
     <row r="581" spans="2:10" ht="15.75" customHeight="1">
+      <c r="B581" s="63"/>
       <c r="J581"/>
     </row>
     <row r="582" spans="2:10" ht="15.75" customHeight="1">
@@ -11794,8 +11818,12 @@
     <row r="980" spans="10:10" ht="15.75" customHeight="1">
       <c r="J980"/>
     </row>
-    <row r="981" spans="10:10" ht="15.75" customHeight="1"/>
-    <row r="982" spans="10:10" ht="15.75" customHeight="1"/>
+    <row r="981" spans="10:10" ht="15.75" customHeight="1">
+      <c r="J981"/>
+    </row>
+    <row r="982" spans="10:10" ht="15.75" customHeight="1">
+      <c r="J982"/>
+    </row>
     <row r="983" spans="10:10" ht="15.75" customHeight="1"/>
     <row r="984" spans="10:10" ht="15.75" customHeight="1"/>
     <row r="985" spans="10:10" ht="15.75" customHeight="1"/>
@@ -11812,23 +11840,71 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A214" r:id="rId1"/>
+    <hyperlink ref="A216" r:id="rId1"/>
     <hyperlink ref="A85" r:id="rId2"/>
     <hyperlink ref="A79" r:id="rId3"/>
     <hyperlink ref="A4" r:id="rId4"/>
     <hyperlink ref="A6" r:id="rId5"/>
     <hyperlink ref="A7" r:id="rId6"/>
     <hyperlink ref="A14" r:id="rId7"/>
+    <hyperlink ref="A215" r:id="rId8"/>
+    <hyperlink ref="A214" r:id="rId9"/>
+    <hyperlink ref="A213" r:id="rId10"/>
+    <hyperlink ref="A212" r:id="rId11"/>
+    <hyperlink ref="A211" r:id="rId12"/>
+    <hyperlink ref="A210" r:id="rId13"/>
+    <hyperlink ref="A209" r:id="rId14"/>
+    <hyperlink ref="A8" r:id="rId15"/>
+    <hyperlink ref="A15" r:id="rId16"/>
+    <hyperlink ref="A16" r:id="rId17"/>
+    <hyperlink ref="A17" r:id="rId18"/>
+    <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A19" r:id="rId20"/>
+    <hyperlink ref="A20" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
+    <hyperlink ref="A23" r:id="rId23"/>
+    <hyperlink ref="A24" r:id="rId24"/>
+    <hyperlink ref="A27" r:id="rId25"/>
+    <hyperlink ref="A28" r:id="rId26"/>
+    <hyperlink ref="A29" r:id="rId27"/>
+    <hyperlink ref="A30" r:id="rId28"/>
+    <hyperlink ref="A49" r:id="rId29"/>
+    <hyperlink ref="A50" r:id="rId30"/>
+    <hyperlink ref="A51" r:id="rId31"/>
+    <hyperlink ref="A54" r:id="rId32"/>
+    <hyperlink ref="A55" r:id="rId33"/>
+    <hyperlink ref="A56" r:id="rId34"/>
+    <hyperlink ref="A58" r:id="rId35"/>
+    <hyperlink ref="A60" r:id="rId36"/>
+    <hyperlink ref="A62" r:id="rId37"/>
+    <hyperlink ref="A64" r:id="rId38"/>
+    <hyperlink ref="A74" r:id="rId39"/>
+    <hyperlink ref="A75" r:id="rId40"/>
+    <hyperlink ref="A77" r:id="rId41"/>
+    <hyperlink ref="A78" r:id="rId42"/>
+    <hyperlink ref="A94" r:id="rId43"/>
+    <hyperlink ref="A96" r:id="rId44"/>
+    <hyperlink ref="A97" r:id="rId45"/>
+    <hyperlink ref="A99" r:id="rId46"/>
+    <hyperlink ref="A100" r:id="rId47"/>
+    <hyperlink ref="A101" r:id="rId48"/>
+    <hyperlink ref="A102" r:id="rId49"/>
+    <hyperlink ref="A205" r:id="rId50"/>
+    <hyperlink ref="A206" r:id="rId51"/>
+    <hyperlink ref="A207" r:id="rId52"/>
+    <hyperlink ref="A208" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId54"/>
+  <drawing r:id="rId55"/>
 </worksheet>
 </file>
 
@@ -11855,50 +11931,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="140" t="s">
         <v>489</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
-      <c r="I1" s="156"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="143" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="142"/>
+      <c r="B2" s="144"/>
       <c r="C2" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D2" s="158" t="s">
+      <c r="D2" s="145" t="s">
         <v>492</v>
       </c>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="159" t="s">
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="147" t="s">
         <v>493</v>
       </c>
-      <c r="I2" s="146"/>
+      <c r="I2" s="148"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="149" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="156"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="142"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="8" t="s">
@@ -11960,15 +12036,15 @@
       <c r="I6" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="K6" s="148" t="s">
+      <c r="K6" s="150" t="s">
         <v>512</v>
       </c>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="149"/>
-      <c r="O6" s="149"/>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="149"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="151"/>
+      <c r="O6" s="151"/>
+      <c r="P6" s="151"/>
+      <c r="Q6" s="151"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="12">
@@ -11998,15 +12074,15 @@
       <c r="I7" s="14" t="s">
         <v>520</v>
       </c>
-      <c r="K7" s="148" t="s">
+      <c r="K7" s="150" t="s">
         <v>521</v>
       </c>
-      <c r="L7" s="149"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="149"/>
-      <c r="O7" s="149"/>
-      <c r="P7" s="149"/>
-      <c r="Q7" s="149"/>
+      <c r="L7" s="151"/>
+      <c r="M7" s="151"/>
+      <c r="N7" s="151"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="151"/>
+      <c r="Q7" s="151"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="12">
@@ -12114,17 +12190,17 @@
       <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="150" t="s">
+      <c r="A15" s="152" t="s">
         <v>530</v>
       </c>
-      <c r="B15" s="151"/>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="152"/>
+      <c r="B15" s="153"/>
+      <c r="C15" s="153"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="153"/>
+      <c r="F15" s="153"/>
+      <c r="G15" s="153"/>
+      <c r="H15" s="153"/>
+      <c r="I15" s="154"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="8" t="s">
@@ -12139,15 +12215,15 @@
       <c r="D16" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="E16" s="153" t="s">
+      <c r="E16" s="155" t="s">
         <v>531</v>
       </c>
-      <c r="F16" s="140"/>
-      <c r="G16" s="153" t="s">
+      <c r="F16" s="156"/>
+      <c r="G16" s="155" t="s">
         <v>532</v>
       </c>
-      <c r="H16" s="143"/>
-      <c r="I16" s="144"/>
+      <c r="H16" s="157"/>
+      <c r="I16" s="158"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="19">
@@ -12162,15 +12238,15 @@
       <c r="D17" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="E17" s="147" t="s">
+      <c r="E17" s="159" t="s">
         <v>534</v>
       </c>
-      <c r="F17" s="140"/>
-      <c r="G17" s="147" t="s">
+      <c r="F17" s="156"/>
+      <c r="G17" s="159" t="s">
         <v>535</v>
       </c>
-      <c r="H17" s="143"/>
-      <c r="I17" s="144"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="158"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="19">
@@ -12185,15 +12261,15 @@
       <c r="D18" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="E18" s="147" t="s">
+      <c r="E18" s="159" t="s">
         <v>534</v>
       </c>
-      <c r="F18" s="140"/>
-      <c r="G18" s="147" t="s">
+      <c r="F18" s="156"/>
+      <c r="G18" s="159" t="s">
         <v>537</v>
       </c>
-      <c r="H18" s="143"/>
-      <c r="I18" s="144"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="158"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="19">
@@ -12208,15 +12284,15 @@
       <c r="D19" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="E19" s="147" t="s">
+      <c r="E19" s="159" t="s">
         <v>540</v>
       </c>
-      <c r="F19" s="140"/>
-      <c r="G19" s="147" t="s">
+      <c r="F19" s="156"/>
+      <c r="G19" s="159" t="s">
         <v>541</v>
       </c>
-      <c r="H19" s="143"/>
-      <c r="I19" s="144"/>
+      <c r="H19" s="157"/>
+      <c r="I19" s="158"/>
       <c r="K19" s="11" t="s">
         <v>542</v>
       </c>
@@ -12228,11 +12304,11 @@
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="139"/>
-      <c r="F20" s="140"/>
-      <c r="G20" s="139"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="144"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="158"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="19">
@@ -12241,11 +12317,11 @@
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="139"/>
-      <c r="F21" s="140"/>
-      <c r="G21" s="139"/>
-      <c r="H21" s="143"/>
-      <c r="I21" s="144"/>
+      <c r="E21" s="160"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="158"/>
       <c r="K21" s="11" t="s">
         <v>543</v>
       </c>
@@ -12257,11 +12333,11 @@
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="144"/>
+      <c r="E22" s="160"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="158"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="19">
@@ -12270,11 +12346,11 @@
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="144"/>
+      <c r="E23" s="160"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="158"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="19">
@@ -12283,11 +12359,11 @@
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="139"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="139"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="144"/>
+      <c r="E24" s="160"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="158"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="19">
@@ -12296,11 +12372,11 @@
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="139"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="144"/>
+      <c r="E25" s="160"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="158"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="21">
@@ -12309,11 +12385,11 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="141"/>
-      <c r="F26" s="142"/>
-      <c r="G26" s="141"/>
-      <c r="H26" s="145"/>
-      <c r="I26" s="146"/>
+      <c r="E26" s="161"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="161"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="148"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -13291,16 +13367,14 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -13313,14 +13387,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -13370,11 +13446,11 @@
       <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="162" t="s">
         <v>546</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="164"/>
       <c r="D2" s="26"/>
       <c r="E2" s="27"/>
       <c r="F2" s="28"/>
@@ -16468,10 +16544,10 @@
   <sheetData>
     <row r="1" spans="2:15" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="165" t="s">
         <v>554</v>
       </c>
-      <c r="C2" s="140"/>
+      <c r="C2" s="156"/>
       <c r="O2" s="11" t="s">
         <v>555</v>
       </c>
@@ -17685,56 +17761,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="165" t="s">
         <v>587</v>
       </c>
-      <c r="B3" s="143"/>
-      <c r="C3" s="140"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="43" t="s">
         <v>495</v>
       </c>
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="167" t="s">
         <v>588</v>
       </c>
-      <c r="C4" s="140"/>
+      <c r="C4" s="156"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="44" t="s">
         <v>589</v>
       </c>
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="166" t="s">
         <v>590</v>
       </c>
-      <c r="C5" s="140"/>
+      <c r="C5" s="156"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="44" t="s">
         <v>591</v>
       </c>
-      <c r="B6" s="165" t="s">
+      <c r="B6" s="166" t="s">
         <v>592</v>
       </c>
-      <c r="C6" s="140"/>
+      <c r="C6" s="156"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="44" t="s">
         <v>593</v>
       </c>
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="166" t="s">
         <v>594</v>
       </c>
-      <c r="C7" s="140"/>
+      <c r="C7" s="156"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="44" t="s">
         <v>595</v>
       </c>
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="166" t="s">
         <v>596</v>
       </c>
-      <c r="C8" s="140"/>
+      <c r="C8" s="156"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -18762,11 +18838,11 @@
       <c r="D1" s="45"/>
     </row>
     <row r="2" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B2" s="167" t="s">
+      <c r="B2" s="168" t="s">
         <v>597</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="156"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="142"/>
       <c r="J2" s="11" t="s">
         <v>555</v>
       </c>
@@ -22915,11 +22991,11 @@
     <row r="3" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="166" t="s">
+      <c r="A5" s="167" t="s">
         <v>630</v>
       </c>
-      <c r="B5" s="143"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="157"/>
+      <c r="C5" s="156"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="43" t="s">

</xml_diff>